<commit_message>
Aggiunta suddivisione per bucket e relativa analisi del pitch
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacopoazzetti/Documents/università/TESI/visual-audio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE82D2A-6110-6B4A-A7F4-359370CC6D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA51F89B-9C56-7040-AE88-712F6D02549B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" xr2:uid="{539C8620-7C30-FF4C-9515-44D5778B2A1D}"/>
   </bookViews>
@@ -1271,7 +1271,7 @@
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
modificate funzioni e commentato meglio
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacopoazzetti/Documents/università/TESI/visual-audio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA51F89B-9C56-7040-AE88-712F6D02549B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156FD5BD-1B20-6145-B558-08D3E47D3901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" xr2:uid="{539C8620-7C30-FF4C-9515-44D5778B2A1D}"/>
   </bookViews>
@@ -22,7 +22,7 @@
     <sheet name="Sorted by Pitch" sheetId="2" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'New Data'!$A$1:$L$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'New Data'!$A$1:$L$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="47">
   <si>
     <t>Song in Exam</t>
   </si>
@@ -176,29 +176,27 @@
     <t>manu chao - bongo bong</t>
   </si>
   <si>
-    <t>Associated Color by Coef</t>
+    <t>Coefficent</t>
   </si>
   <si>
-    <t>My idea of Association</t>
+    <t>Sons Of The East - Into The Sun</t>
   </si>
   <si>
-    <t>↑</t>
+    <t>Duration (sec.)</t>
   </si>
   <si>
-    <t>↓</t>
-  </si>
-  <si>
-    <t>Another CF</t>
+    <t>Energy per Sec</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.00000000000"/>
+    <numFmt numFmtId="172" formatCode="0.00000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -238,7 +236,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -355,114 +353,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF3E33"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFE883B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFBA40"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEFBF43"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD6C03F"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBBC63F"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8ACB48"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7BCF6A"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF65D696"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF46DAC5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF10E2F9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF1BC6FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF1FB9FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF299AFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF2D87FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8C6FFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7FD76F"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -489,7 +385,7 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -507,12 +403,16 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -521,27 +421,38 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
+      <top style="medium">
         <color indexed="64"/>
-      </bottom>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -608,87 +519,25 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -721,70 +570,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>116417</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>211666</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>746335</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>14393</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Immagine 1" descr="Gradient Tool - Pixelmator Classic Tutorials">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABF4CE59-4CA5-2E48-9468-8746B8247343}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="21655"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm rot="16200000">
-          <a:off x="15854679" y="1703071"/>
-          <a:ext cx="3612727" cy="629918"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -907,7 +692,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1268,69 +1053,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D881CB1C-05FC-3146-9C78-C0AA3598EAD0}">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="44.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.83203125" customWidth="1"/>
-    <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="34" t="s">
+      <c r="B1" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" s="72" t="s">
-        <v>47</v>
-      </c>
-      <c r="L1" s="53" t="s">
+      <c r="J1" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="54" t="s">
-        <v>44</v>
+      <c r="K1" s="38" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="3">
+      <c r="B2" s="40">
+        <v>312</v>
+      </c>
+      <c r="C2" s="41">
         <v>123.05</v>
       </c>
       <c r="D2">
@@ -1342,7 +1128,7 @@
       <c r="F2" s="3">
         <v>1831000.875</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="41">
         <v>1837.5</v>
       </c>
       <c r="H2" t="s">
@@ -1352,338 +1138,352 @@
         <v>1.3644000000000001</v>
       </c>
       <c r="J2" s="3">
-        <v>3364464107.8099999</v>
-      </c>
-      <c r="K2" s="16">
-        <f>+(F2/C2)-(F2/G2)</f>
-        <v>13883.67407814975</v>
-      </c>
-      <c r="L2" s="36"/>
-      <c r="N2" s="55"/>
-      <c r="P2" s="16">
-        <f>K2/10000000</f>
-        <v>1.3883674078149751E-3</v>
-      </c>
+        <v>13884.05</v>
+      </c>
+      <c r="K2" s="41">
+        <f>F2/B2</f>
+        <v>5868.5925480769229</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="3">
-        <v>129.19999999999999</v>
+        <v>25</v>
+      </c>
+      <c r="B3" s="40">
+        <v>190</v>
+      </c>
+      <c r="C3" s="41">
+        <v>123.05</v>
       </c>
       <c r="D3">
-        <v>0.1777</v>
+        <v>0.18410000000000001</v>
       </c>
       <c r="E3">
-        <v>-11.209899999999999</v>
+        <v>-10.3398</v>
       </c>
       <c r="F3" s="3">
-        <v>1677930.375</v>
-      </c>
-      <c r="G3" s="3">
-        <v>294</v>
+        <v>921989.5</v>
+      </c>
+      <c r="G3" s="41">
+        <v>816.67</v>
       </c>
       <c r="H3" t="s">
         <v>10</v>
       </c>
       <c r="I3">
-        <v>1.7843</v>
+        <v>1.1934</v>
       </c>
       <c r="J3" s="3">
-        <v>493311530.25</v>
-      </c>
-      <c r="K3" s="16">
         <f>+(F3/C3)-(F3/G3)</f>
-        <v>7279.831032412967</v>
-      </c>
-      <c r="L3" s="39"/>
-      <c r="N3" s="56"/>
-      <c r="P3" s="16">
-        <f t="shared" ref="P3:P18" si="0">K3/10000000</f>
-        <v>7.2798310324129667E-4</v>
-      </c>
+        <v>6363.8416116325598</v>
+      </c>
+      <c r="K3" s="41">
+        <f>F3/B3</f>
+        <v>4852.5763157894735</v>
+      </c>
+      <c r="L3" s="3">
+        <f>+K3+C3+G3</f>
+        <v>5792.2963157894737</v>
+      </c>
+      <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="3">
-        <v>89.1</v>
+        <v>23</v>
+      </c>
+      <c r="B4" s="40">
+        <v>297</v>
+      </c>
+      <c r="C4" s="41">
+        <v>112.35</v>
       </c>
       <c r="D4">
-        <v>0.1426</v>
+        <v>0.1118</v>
       </c>
       <c r="E4">
-        <v>-12.9703</v>
+        <v>-12.9529</v>
       </c>
       <c r="F4" s="3">
-        <v>756879.875</v>
-      </c>
-      <c r="G4" s="3">
-        <v>580.26</v>
+        <v>706575.5</v>
+      </c>
+      <c r="G4" s="41">
+        <v>2004.55</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I4">
-        <v>1.0942000000000001</v>
+        <v>1.2081999999999999</v>
       </c>
       <c r="J4" s="3">
-        <v>439189506.41000003</v>
-      </c>
-      <c r="K4" s="16">
-        <f>+(F4/C4)-(F4/G4)</f>
-        <v>7190.3430457448485</v>
-      </c>
-      <c r="L4" s="40"/>
-      <c r="N4" s="57"/>
-      <c r="P4" s="16">
-        <f t="shared" si="0"/>
-        <v>7.190343045744849E-4</v>
-      </c>
+        <v>5936.73</v>
+      </c>
+      <c r="K4" s="41">
+        <f>F4/B4</f>
+        <v>2379.0420875420878</v>
+      </c>
+      <c r="L4" s="3">
+        <f>+K4+C4+G4</f>
+        <v>4495.9420875420874</v>
+      </c>
+      <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="3">
-        <v>123.05</v>
+        <v>31</v>
+      </c>
+      <c r="B5" s="40">
+        <v>427</v>
+      </c>
+      <c r="C5" s="41">
+        <v>129.19999999999999</v>
       </c>
       <c r="D5">
-        <v>0.18410000000000001</v>
+        <v>0.1777</v>
       </c>
       <c r="E5">
-        <v>-10.3398</v>
+        <v>-11.209899999999999</v>
       </c>
       <c r="F5" s="3">
-        <v>921989.5</v>
-      </c>
-      <c r="G5" s="3">
-        <v>816.67</v>
+        <v>1677930.375</v>
+      </c>
+      <c r="G5" s="41">
+        <v>294</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
       </c>
       <c r="I5">
-        <v>1.1934</v>
+        <v>1.7843</v>
       </c>
       <c r="J5" s="3">
-        <v>752958091.66999996</v>
-      </c>
-      <c r="K5" s="16">
-        <f>+(F5/C5)-(F5/G5)</f>
-        <v>6363.8416116325598</v>
-      </c>
-      <c r="L5" s="38"/>
-      <c r="N5" s="58"/>
-      <c r="P5" s="16">
-        <f t="shared" si="0"/>
-        <v>6.3638416116325596E-4</v>
-      </c>
+        <v>7279.91</v>
+      </c>
+      <c r="K5" s="41">
+        <f>F5/B5</f>
+        <v>3929.5793325526934</v>
+      </c>
+      <c r="L5" s="3">
+        <f>+K5+C5+G5</f>
+        <v>4352.7793325526927</v>
+      </c>
+      <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="3">
-        <v>112.35</v>
+        <v>42</v>
+      </c>
+      <c r="B6" s="40">
+        <v>158</v>
+      </c>
+      <c r="C6" s="41">
+        <v>152</v>
       </c>
       <c r="D6">
-        <v>0.1118</v>
+        <v>0.15329999999999999</v>
       </c>
       <c r="E6">
-        <v>-12.9529</v>
+        <v>-11.6812</v>
       </c>
       <c r="F6" s="3">
-        <v>706575.5</v>
-      </c>
-      <c r="G6" s="3">
-        <v>2004.55</v>
+        <v>514259.3125</v>
+      </c>
+      <c r="G6" s="41">
+        <v>297.97000000000003</v>
       </c>
       <c r="H6" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="I6">
-        <v>1.2081999999999999</v>
+        <v>1.4330000000000001</v>
       </c>
       <c r="J6" s="3">
-        <v>1416362706.8199999</v>
-      </c>
-      <c r="K6" s="16">
-        <f>+(F6/C6)-(F6/G6)</f>
-        <v>5936.5706751008838</v>
-      </c>
-      <c r="L6" s="37"/>
-      <c r="N6" s="59"/>
-      <c r="P6" s="16">
-        <f t="shared" si="0"/>
-        <v>5.9365706751008838E-4</v>
-      </c>
+        <v>1657.45</v>
+      </c>
+      <c r="K6" s="41">
+        <f>F6/B6</f>
+        <v>3254.8057753164558</v>
+      </c>
+      <c r="L6" s="3">
+        <f>+K6+C6+G6</f>
+        <v>3704.775775316456</v>
+      </c>
+      <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="40">
+        <v>265</v>
+      </c>
+      <c r="C7" s="41">
+        <v>89.1</v>
+      </c>
+      <c r="D7">
+        <v>0.1426</v>
+      </c>
+      <c r="E7">
+        <v>-12.9703</v>
+      </c>
+      <c r="F7" s="3">
+        <v>756879.875</v>
+      </c>
+      <c r="G7" s="41">
+        <v>580.26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7">
+        <v>1.0942000000000001</v>
+      </c>
+      <c r="J7" s="3">
+        <v>7190.07</v>
+      </c>
+      <c r="K7" s="41">
+        <f>F7/B7</f>
+        <v>2856.1504716981131</v>
+      </c>
+      <c r="L7" s="3">
+        <f>+K7+C7+G7</f>
+        <v>3525.5104716981132</v>
+      </c>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="3">
+      <c r="B8" s="40">
+        <v>234</v>
+      </c>
+      <c r="C8" s="41">
         <v>83.35</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <v>0.1225</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>-13.845499999999999</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F8" s="3">
         <v>563190.75</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G8" s="41">
         <v>648.53</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H8" t="s">
         <v>15</v>
       </c>
-      <c r="I7">
+      <c r="I8">
         <v>1.5992</v>
       </c>
-      <c r="J7" s="3">
-        <v>365245765.81</v>
-      </c>
-      <c r="K7" s="16">
-        <f>+(F7/C7)-(F7/G7)</f>
-        <v>5888.5263593357849</v>
-      </c>
-      <c r="L7" s="41"/>
-      <c r="N7" s="60"/>
-      <c r="P7" s="16">
-        <f t="shared" si="0"/>
-        <v>5.8885263593357853E-4</v>
-      </c>
+      <c r="J8" s="3">
+        <v>5888.17</v>
+      </c>
+      <c r="K8" s="41">
+        <f>F8/B8</f>
+        <v>2406.7980769230771</v>
+      </c>
+      <c r="L8" s="3">
+        <f>+K8+C8+G8</f>
+        <v>3138.6780769230772</v>
+      </c>
+      <c r="N8" s="3"/>
     </row>
-    <row r="8" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="3">
-        <v>112.35</v>
-      </c>
-      <c r="D8">
-        <v>0.1172</v>
-      </c>
-      <c r="E8">
-        <v>-14.929500000000001</v>
-      </c>
-      <c r="F8" s="3">
-        <v>1129507.5</v>
-      </c>
-      <c r="G8" s="3">
-        <v>165.79</v>
-      </c>
-      <c r="H8" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="40">
+        <v>158</v>
+      </c>
+      <c r="C9" s="41">
+        <v>129.19999999999999</v>
+      </c>
+      <c r="D9">
+        <v>0.1318</v>
+      </c>
+      <c r="E9">
+        <v>-13.7721</v>
+      </c>
+      <c r="F9" s="3">
+        <v>416358.8125</v>
+      </c>
+      <c r="G9" s="41">
+        <v>339.23</v>
+      </c>
+      <c r="H9" t="s">
         <v>30</v>
       </c>
-      <c r="I8">
-        <v>1.4455</v>
-      </c>
-      <c r="J8" s="3">
-        <v>187260453.94999999</v>
-      </c>
-      <c r="K8" s="16">
-        <f>+(F8/C8)-(F8/G8)</f>
-        <v>3240.5905423005652</v>
-      </c>
-      <c r="L8" s="45"/>
-      <c r="N8" s="61"/>
-      <c r="P8" s="16">
-        <f t="shared" si="0"/>
-        <v>3.240590542300565E-4</v>
-      </c>
+      <c r="I9">
+        <v>1.1842999999999999</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1995.25</v>
+      </c>
+      <c r="K9" s="41">
+        <f>F9/B9</f>
+        <v>2635.1823575949365</v>
+      </c>
+      <c r="L9" s="3">
+        <f>+K9+C9+G9</f>
+        <v>3103.6123575949364</v>
+      </c>
+      <c r="N9" s="3"/>
     </row>
-    <row r="9" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="3">
+      <c r="B10" s="40">
+        <v>238</v>
+      </c>
+      <c r="C10" s="41">
         <v>136</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>0.13439999999999999</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <v>-14.295199999999999</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F10" s="3">
         <v>603749.3125</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G10" s="41">
         <v>408.33</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H10" t="s">
         <v>10</v>
       </c>
-      <c r="I9">
+      <c r="I10">
         <v>1.0834999999999999</v>
       </c>
-      <c r="J9" s="3">
-        <v>246530969.27000001</v>
-      </c>
-      <c r="K9" s="16">
-        <f>+(F9/C9)-(F9/G9)</f>
-        <v>2960.7513651934669</v>
-      </c>
-      <c r="L9" s="43"/>
-      <c r="N9" s="71" t="s">
-        <v>46</v>
-      </c>
-      <c r="P9" s="16">
-        <f t="shared" si="0"/>
-        <v>2.9607513651934669E-4</v>
-      </c>
+      <c r="J10" s="3">
+        <v>2960.79</v>
+      </c>
+      <c r="K10" s="41">
+        <f>F10/B10</f>
+        <v>2536.7618172268908</v>
+      </c>
+      <c r="L10" s="3">
+        <f>+K10+C10+G10</f>
+        <v>3081.0918172268907</v>
+      </c>
+      <c r="N10" s="3"/>
     </row>
-    <row r="10" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="3">
-        <v>78.3</v>
-      </c>
-      <c r="D10">
-        <v>8.48E-2</v>
-      </c>
-      <c r="E10">
-        <v>-16.337700000000002</v>
-      </c>
-      <c r="F10" s="3">
-        <v>237987.46875</v>
-      </c>
-      <c r="G10" s="3">
-        <v>816.67</v>
-      </c>
-      <c r="H10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10">
-        <v>1.1517999999999999</v>
-      </c>
-      <c r="J10" s="3">
-        <v>194356432.81</v>
-      </c>
-      <c r="K10" s="16">
-        <f>+(F10/C10)-(F10/G10)</f>
-        <v>2748.0192363424321</v>
-      </c>
-      <c r="L10" s="44"/>
-      <c r="N10" s="62"/>
-      <c r="P10" s="16">
-        <f t="shared" si="0"/>
-        <v>2.7480192363424323E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3">
+      <c r="B11" s="40">
+        <v>232</v>
+      </c>
+      <c r="C11" s="41">
         <v>161.5</v>
       </c>
       <c r="D11">
@@ -1695,7 +1495,7 @@
       <c r="F11" s="3">
         <v>504097.78125</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="41">
         <v>551.25</v>
       </c>
       <c r="H11" t="s">
@@ -1705,24 +1505,26 @@
         <v>1.387</v>
       </c>
       <c r="J11" s="3">
-        <v>277883901.91000003</v>
-      </c>
-      <c r="K11" s="16">
-        <f>+(F11/C11)-(F11/G11)</f>
-        <v>2206.8853954739789</v>
-      </c>
-      <c r="L11" s="42"/>
-      <c r="N11" s="63"/>
-      <c r="P11" s="16">
-        <f t="shared" si="0"/>
-        <v>2.2068853954739789E-4</v>
-      </c>
+        <v>2206.9</v>
+      </c>
+      <c r="K11" s="41">
+        <f>F11/B11</f>
+        <v>2172.8352640086205</v>
+      </c>
+      <c r="L11" s="3">
+        <f>+K11+C11+G11</f>
+        <v>2885.5852640086205</v>
+      </c>
+      <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="3">
+      <c r="B12" s="40">
+        <v>104</v>
+      </c>
+      <c r="C12" s="41">
         <v>92.29</v>
       </c>
       <c r="D12">
@@ -1734,7 +1536,7 @@
       <c r="F12" s="3">
         <v>233933.890625</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="41">
         <v>512.79</v>
       </c>
       <c r="H12" t="s">
@@ -1744,270 +1546,316 @@
         <v>1.1315999999999999</v>
       </c>
       <c r="J12" s="3">
-        <v>119959122.98</v>
-      </c>
-      <c r="K12" s="16">
-        <f>+(F12/C12)-(F12/G12)</f>
-        <v>2078.5714154395087</v>
-      </c>
-      <c r="L12" s="48"/>
-      <c r="N12" s="65" t="s">
-        <v>45</v>
-      </c>
-      <c r="P12" s="16">
-        <f t="shared" si="0"/>
-        <v>2.0785714154395086E-4</v>
-      </c>
+        <v>2078.71</v>
+      </c>
+      <c r="K12" s="41">
+        <f>F12/B12</f>
+        <v>2249.3643329326924</v>
+      </c>
+      <c r="L12" s="3">
+        <f>+K12+C12+G12</f>
+        <v>2854.4443329326923</v>
+      </c>
+      <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="3">
-        <v>129.19999999999999</v>
+        <v>35</v>
+      </c>
+      <c r="B13" s="40">
+        <v>544</v>
+      </c>
+      <c r="C13" s="41">
+        <v>112.35</v>
       </c>
       <c r="D13">
-        <v>0.1318</v>
+        <v>0.1172</v>
       </c>
       <c r="E13">
-        <v>-13.7721</v>
+        <v>-14.929500000000001</v>
       </c>
       <c r="F13" s="3">
-        <v>416358.8125</v>
-      </c>
-      <c r="G13" s="3">
-        <v>339.23</v>
+        <v>1129507.5</v>
+      </c>
+      <c r="G13" s="41">
+        <v>165.79</v>
       </c>
       <c r="H13" t="s">
         <v>30</v>
       </c>
       <c r="I13">
-        <v>1.1842999999999999</v>
+        <v>1.4455</v>
       </c>
       <c r="J13" s="3">
-        <v>141241720.24000001</v>
-      </c>
-      <c r="K13" s="16">
-        <f>+(F13/C13)-(F13/G13)</f>
-        <v>1995.2270660812476</v>
-      </c>
-      <c r="L13" s="47"/>
-      <c r="N13" s="66"/>
-      <c r="P13" s="16">
-        <f t="shared" si="0"/>
-        <v>1.9952270660812476E-4</v>
-      </c>
+        <v>3240.82</v>
+      </c>
+      <c r="K13" s="41">
+        <f>F13/B13</f>
+        <v>2076.3005514705883</v>
+      </c>
+      <c r="L13" s="3">
+        <f>+K13+C13+G13</f>
+        <v>2354.4405514705882</v>
+      </c>
+      <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="3">
+        <v>44</v>
+      </c>
+      <c r="B14" s="40">
+        <v>293</v>
+      </c>
+      <c r="C14" s="40">
+        <v>112.35</v>
+      </c>
+      <c r="D14">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="E14">
+        <v>-15.7897</v>
+      </c>
+      <c r="F14" s="3">
+        <v>326635.5625</v>
+      </c>
+      <c r="G14" s="40">
+        <v>689.06</v>
+      </c>
+      <c r="H14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14">
+        <v>0.93610000000000004</v>
+      </c>
+      <c r="J14">
+        <v>2433.35</v>
+      </c>
+      <c r="K14" s="41">
+        <f>F14/B14</f>
+        <v>1114.7971416382252</v>
+      </c>
+      <c r="L14" s="3">
+        <f>+K14+C14+G14</f>
+        <v>1916.207141638225</v>
+      </c>
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="40">
+        <v>237</v>
+      </c>
+      <c r="C15" s="41">
+        <v>78.3</v>
+      </c>
+      <c r="D15">
+        <v>8.48E-2</v>
+      </c>
+      <c r="E15">
+        <v>-16.337700000000002</v>
+      </c>
+      <c r="F15" s="3">
+        <v>237987.46875</v>
+      </c>
+      <c r="G15" s="41">
+        <v>816.67</v>
+      </c>
+      <c r="H15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15">
+        <v>1.1517999999999999</v>
+      </c>
+      <c r="J15" s="3">
+        <v>2747.92</v>
+      </c>
+      <c r="K15" s="41">
+        <f>F15/B15</f>
+        <v>1004.1665348101266</v>
+      </c>
+      <c r="L15" s="3">
+        <f>+K15+C15+G15</f>
+        <v>1899.1365348101267</v>
+      </c>
+      <c r="N15" s="3"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="40">
+        <v>65</v>
+      </c>
+      <c r="C16" s="41">
+        <v>117.45</v>
+      </c>
+      <c r="D16">
+        <v>7.6600000000000001E-2</v>
+      </c>
+      <c r="E16">
+        <v>-18.4603</v>
+      </c>
+      <c r="F16" s="3">
+        <v>56900.1796875</v>
+      </c>
+      <c r="G16" s="41">
+        <v>250.57</v>
+      </c>
+      <c r="H16" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16">
+        <v>0.872</v>
+      </c>
+      <c r="J16" s="3">
+        <v>257.36</v>
+      </c>
+      <c r="K16" s="41">
+        <f>F16/B16</f>
+        <v>875.38737980769235</v>
+      </c>
+      <c r="L16" s="3">
+        <f>+K16+C16+G16</f>
+        <v>1243.4073798076925</v>
+      </c>
+      <c r="N16" s="3"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="40">
+        <v>163</v>
+      </c>
+      <c r="C17" s="41">
+        <v>112.35</v>
+      </c>
+      <c r="D17">
+        <v>6.5699999999999995E-2</v>
+      </c>
+      <c r="E17">
+        <v>-18.613099999999999</v>
+      </c>
+      <c r="F17" s="3">
+        <v>99084.421875</v>
+      </c>
+      <c r="G17" s="41">
+        <v>479.35</v>
+      </c>
+      <c r="H17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17">
+        <v>1.0147999999999999</v>
+      </c>
+      <c r="J17" s="3">
+        <v>675.24</v>
+      </c>
+      <c r="K17" s="41">
+        <f>F17/B17</f>
+        <v>607.87988880368096</v>
+      </c>
+      <c r="L17" s="3">
+        <f>+K17+C17+G17</f>
+        <v>1199.5798888036811</v>
+      </c>
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="40">
+        <v>284</v>
+      </c>
+      <c r="C18" s="42">
+        <v>129.19999999999999</v>
+      </c>
+      <c r="D18">
+        <v>5.2299999999999999E-2</v>
+      </c>
+      <c r="E18">
+        <v>-18.380500000000001</v>
+      </c>
+      <c r="F18" s="3">
+        <v>143452.09375</v>
+      </c>
+      <c r="G18" s="41">
+        <v>512.79</v>
+      </c>
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18">
+        <v>0.98119999999999996</v>
+      </c>
+      <c r="J18" s="3">
+        <v>830.57</v>
+      </c>
+      <c r="K18" s="41">
+        <f>F18/B18</f>
+        <v>505.11300616197184</v>
+      </c>
+      <c r="L18" s="3">
+        <f>+K18+C18+G18</f>
+        <v>1147.1030061619717</v>
+      </c>
+      <c r="N18" s="3"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="40">
+        <v>273</v>
+      </c>
+      <c r="C19" s="42">
         <v>152</v>
       </c>
-      <c r="D14">
-        <v>0.15329999999999999</v>
-      </c>
-      <c r="E14">
-        <v>-11.6812</v>
-      </c>
-      <c r="F14" s="3">
-        <v>514259.3125</v>
-      </c>
-      <c r="G14" s="3">
-        <v>297.97000000000003</v>
-      </c>
-      <c r="H14" t="s">
-        <v>30</v>
-      </c>
-      <c r="I14">
-        <v>1.4330000000000001</v>
-      </c>
-      <c r="J14" s="3">
-        <v>153235376.22</v>
-      </c>
-      <c r="K14" s="16">
-        <f>+(F14/C14)-(F14/G14)</f>
-        <v>1657.4088137984793</v>
-      </c>
-      <c r="L14" s="46"/>
-      <c r="N14" s="67" t="s">
-        <v>45</v>
-      </c>
-      <c r="P14" s="16">
-        <f t="shared" si="0"/>
-        <v>1.6574088137984793E-4</v>
-      </c>
+      <c r="D19">
+        <v>4.7800000000000002E-2</v>
+      </c>
+      <c r="E19">
+        <v>-20.896899999999999</v>
+      </c>
+      <c r="F19" s="3">
+        <v>114231.59375</v>
+      </c>
+      <c r="G19" s="41">
+        <v>256.39999999999998</v>
+      </c>
+      <c r="H19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19">
+        <v>1.2103999999999999</v>
+      </c>
+      <c r="J19" s="3">
+        <v>306</v>
+      </c>
+      <c r="K19" s="41">
+        <f>F19/B19</f>
+        <v>418.43074633699632</v>
+      </c>
+      <c r="L19" s="3">
+        <f>+K19+C19+G19</f>
+        <v>826.8307463369963</v>
+      </c>
+      <c r="M19" s="37"/>
+      <c r="N19" s="3"/>
     </row>
-    <row r="15" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="35">
-        <v>129.19999999999999</v>
-      </c>
-      <c r="D15">
-        <v>5.2299999999999999E-2</v>
-      </c>
-      <c r="E15">
-        <v>-18.380500000000001</v>
-      </c>
-      <c r="F15" s="3">
-        <v>143452.09375</v>
-      </c>
-      <c r="G15" s="3">
-        <v>512.79</v>
-      </c>
-      <c r="H15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15">
-        <v>0.98119999999999996</v>
-      </c>
-      <c r="J15" s="3">
-        <v>73560899.239999995</v>
-      </c>
-      <c r="K15" s="16">
-        <f>+(F15/C15)-(F15/G15)</f>
-        <v>830.56209531035893</v>
-      </c>
-      <c r="L15" s="49"/>
-      <c r="N15" s="68"/>
-      <c r="P15" s="16">
-        <f t="shared" si="0"/>
-        <v>8.3056209531035899E-5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="3">
-        <v>112.35</v>
-      </c>
-      <c r="D16">
-        <v>6.5699999999999995E-2</v>
-      </c>
-      <c r="E16">
-        <v>-18.613099999999999</v>
-      </c>
-      <c r="F16" s="3">
-        <v>99084.421875</v>
-      </c>
-      <c r="G16" s="3">
-        <v>479.35</v>
-      </c>
-      <c r="H16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16">
-        <v>1.0147999999999999</v>
-      </c>
-      <c r="J16" s="3">
-        <v>47495902.219999999</v>
-      </c>
-      <c r="K16" s="16">
-        <f>+(F16/C16)-(F16/G16)</f>
-        <v>675.22052542362735</v>
-      </c>
-      <c r="L16" s="50"/>
-      <c r="N16" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="P16" s="16">
-        <f t="shared" si="0"/>
-        <v>6.7522052542362735E-5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="35">
-        <v>152</v>
-      </c>
-      <c r="D17">
-        <v>4.7800000000000002E-2</v>
-      </c>
-      <c r="E17">
-        <v>-20.896899999999999</v>
-      </c>
-      <c r="F17" s="3">
-        <v>114231.59375</v>
-      </c>
-      <c r="G17" s="3">
-        <v>256.39999999999998</v>
-      </c>
-      <c r="H17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I17">
-        <v>1.2103999999999999</v>
-      </c>
-      <c r="J17" s="3">
-        <v>29288449.329999998</v>
-      </c>
-      <c r="K17" s="16">
-        <f>+(F17/C17)-(F17/G17)</f>
-        <v>306.00260662564659</v>
-      </c>
-      <c r="L17" s="51"/>
-      <c r="N17" s="70"/>
-      <c r="P17" s="16">
-        <f t="shared" si="0"/>
-        <v>3.0600260662564658E-5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="3">
-        <v>117.45</v>
-      </c>
-      <c r="D18">
-        <v>7.6600000000000001E-2</v>
-      </c>
-      <c r="E18">
-        <v>-18.4603</v>
-      </c>
-      <c r="F18" s="3">
-        <v>56900.1796875</v>
-      </c>
-      <c r="G18" s="3">
-        <v>250.57</v>
-      </c>
-      <c r="H18" t="s">
-        <v>18</v>
-      </c>
-      <c r="I18">
-        <v>0.872</v>
-      </c>
-      <c r="J18" s="3">
-        <v>14257374.57</v>
-      </c>
-      <c r="K18" s="16">
-        <f>+(F18/C18)-(F18/G18)</f>
-        <v>257.38003329420417</v>
-      </c>
-      <c r="L18" s="52"/>
-      <c r="N18" s="64"/>
-      <c r="P18" s="16">
-        <f t="shared" si="0"/>
-        <v>2.5738003329420418E-5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="K23" s="16"/>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J23" s="16"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L18" xr:uid="{D881CB1C-05FC-3146-9C78-C0AA3598EAD0}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L18">
-      <sortCondition descending="1" ref="K1:K18"/>
+  <autoFilter ref="A1:L19" xr:uid="{D881CB1C-05FC-3146-9C78-C0AA3598EAD0}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L19">
+      <sortCondition descending="1" ref="L1:L19"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2016,7 +1864,7 @@
   <dimension ref="A1:XFB102"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
prima versione del colore in funzione del tempo - da sistemare
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacopoazzetti/Documents/università/TESI/visual-audio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156FD5BD-1B20-6145-B558-08D3E47D3901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7F9E57-F9E6-2944-8423-F77A122BDF97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" xr2:uid="{539C8620-7C30-FF4C-9515-44D5778B2A1D}"/>
   </bookViews>
@@ -22,7 +22,7 @@
     <sheet name="Sorted by Pitch" sheetId="2" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'New Data'!$A$1:$L$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'New Data'!$A$1:$N$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -185,18 +185,17 @@
     <t>Duration (sec.)</t>
   </si>
   <si>
-    <t>Energy per Sec</t>
+    <t>Time Energy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.00000000000"/>
-    <numFmt numFmtId="172" formatCode="0.00000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -528,7 +527,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -538,6 +536,7 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1053,10 +1052,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D881CB1C-05FC-3146-9C78-C0AA3598EAD0}">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1071,17 +1070,18 @@
     <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="38" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="35" t="s">
@@ -1093,7 +1093,7 @@
       <c r="F1" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="38" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="35" t="s">
@@ -1105,18 +1105,18 @@
       <c r="J1" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="38" t="s">
+      <c r="K1" s="37" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="40">
+      <c r="B2" s="39">
         <v>312</v>
       </c>
-      <c r="C2" s="41">
+      <c r="C2" s="40">
         <v>123.05</v>
       </c>
       <c r="D2">
@@ -1128,7 +1128,7 @@
       <c r="F2" s="3">
         <v>1831000.875</v>
       </c>
-      <c r="G2" s="41">
+      <c r="G2" s="40">
         <v>1837.5</v>
       </c>
       <c r="H2" t="s">
@@ -1140,21 +1140,35 @@
       <c r="J2" s="3">
         <v>13884.05</v>
       </c>
-      <c r="K2" s="41">
+      <c r="K2" s="40">
         <f>F2/B2</f>
         <v>5868.5925480769229</v>
       </c>
-      <c r="L2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="L2" s="3">
+        <f>(K2/G2)+(K2/E2)</f>
+        <v>-584.41760553346057</v>
+      </c>
+      <c r="M2" s="3">
+        <f>(K2/G2)+(K2/C2)</f>
+        <v>50.886539104483099</v>
+      </c>
+      <c r="N2" s="3">
+        <f>((K2/G2)+(K2/C2*B2))</f>
+        <v>14883.330931237137</v>
+      </c>
+      <c r="P2" s="42">
+        <f>(G2)/200</f>
+        <v>9.1875</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="40">
+      <c r="B3" s="39">
         <v>190</v>
       </c>
-      <c r="C3" s="41">
+      <c r="C3" s="40">
         <v>123.05</v>
       </c>
       <c r="D3">
@@ -1166,7 +1180,7 @@
       <c r="F3" s="3">
         <v>921989.5</v>
       </c>
-      <c r="G3" s="41">
+      <c r="G3" s="40">
         <v>816.67</v>
       </c>
       <c r="H3" t="s">
@@ -1179,516 +1193,659 @@
         <f>+(F3/C3)-(F3/G3)</f>
         <v>6363.8416116325598</v>
       </c>
-      <c r="K3" s="41">
+      <c r="K3" s="40">
         <f>F3/B3</f>
         <v>4852.5763157894735</v>
       </c>
       <c r="L3" s="3">
-        <f>+K3+C3+G3</f>
-        <v>5792.2963157894737</v>
-      </c>
-      <c r="N3" s="3"/>
+        <f>(K3/G3)+(K3/E3)</f>
+        <v>-463.36855614763004</v>
+      </c>
+      <c r="M3" s="3">
+        <f>(K3/G3)+(K3/C3)</f>
+        <v>45.377715078962922</v>
+      </c>
+      <c r="N3" s="3">
+        <f>((K3/G3)+(K3/C3*B3))</f>
+        <v>7498.7456442476796</v>
+      </c>
+      <c r="P3" s="42">
+        <f t="shared" ref="P3:P19" si="0">(G3)/200</f>
+        <v>4.0833499999999994</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="40">
-        <v>297</v>
-      </c>
-      <c r="C4" s="41">
+        <v>31</v>
+      </c>
+      <c r="B4" s="39">
+        <v>427</v>
+      </c>
+      <c r="C4" s="40">
+        <v>129.19999999999999</v>
+      </c>
+      <c r="D4">
+        <v>0.1777</v>
+      </c>
+      <c r="E4">
+        <v>-11.209899999999999</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1677930.375</v>
+      </c>
+      <c r="G4" s="40">
+        <v>294</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <v>1.7843</v>
+      </c>
+      <c r="J4" s="3">
+        <v>7279.91</v>
+      </c>
+      <c r="K4" s="40">
+        <f>F4/B4</f>
+        <v>3929.5793325526934</v>
+      </c>
+      <c r="L4" s="3">
+        <f>(K4/G4)+(K4/E4)</f>
+        <v>-337.17952432185928</v>
+      </c>
+      <c r="M4" s="3">
+        <f>(K4/G4)+(K4/C4)</f>
+        <v>43.780616813470125</v>
+      </c>
+      <c r="N4" s="3">
+        <f>((K4/G4)+(K4/C4*B4))</f>
+        <v>13000.443121979473</v>
+      </c>
+      <c r="P4" s="42">
+        <f t="shared" si="0"/>
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="39">
+        <v>265</v>
+      </c>
+      <c r="C5" s="40">
+        <v>89.1</v>
+      </c>
+      <c r="D5">
+        <v>0.1426</v>
+      </c>
+      <c r="E5">
+        <v>-12.9703</v>
+      </c>
+      <c r="F5" s="3">
+        <v>756879.875</v>
+      </c>
+      <c r="G5" s="40">
+        <v>580.26</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5">
+        <v>1.0942000000000001</v>
+      </c>
+      <c r="J5" s="3">
+        <v>7190.07</v>
+      </c>
+      <c r="K5" s="40">
+        <f>F5/B5</f>
+        <v>2856.1504716981131</v>
+      </c>
+      <c r="L5" s="3">
+        <f>(K5/G5)+(K5/E5)</f>
+        <v>-215.28477980566842</v>
+      </c>
+      <c r="M5" s="3">
+        <f>(K5/G5)+(K5/C5)</f>
+        <v>36.977751715229189</v>
+      </c>
+      <c r="N5" s="3">
+        <f>((K5/G5)+(K5/C5*B5))</f>
+        <v>8499.6458160059356</v>
+      </c>
+      <c r="P5" s="42">
+        <f t="shared" si="0"/>
+        <v>2.9013</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="39">
+        <v>234</v>
+      </c>
+      <c r="C6" s="40">
+        <v>83.35</v>
+      </c>
+      <c r="D6">
+        <v>0.1225</v>
+      </c>
+      <c r="E6">
+        <v>-13.845499999999999</v>
+      </c>
+      <c r="F6" s="3">
+        <v>563190.75</v>
+      </c>
+      <c r="G6" s="40">
+        <v>648.53</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6">
+        <v>1.5992</v>
+      </c>
+      <c r="J6" s="3">
+        <v>5888.17</v>
+      </c>
+      <c r="K6" s="40">
+        <f>F6/B6</f>
+        <v>2406.7980769230771</v>
+      </c>
+      <c r="L6" s="3">
+        <f>(K6/G6)+(K6/E6)</f>
+        <v>-170.12135511171559</v>
+      </c>
+      <c r="M6" s="3">
+        <f>(K6/G6)+(K6/C6)</f>
+        <v>32.586960964184726</v>
+      </c>
+      <c r="N6" s="3">
+        <f>((K6/G6)+(K6/C6*B6))</f>
+        <v>6760.6487716789661</v>
+      </c>
+      <c r="P6" s="42">
+        <f t="shared" si="0"/>
+        <v>3.2426499999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="39">
+        <v>158</v>
+      </c>
+      <c r="C7" s="40">
+        <v>152</v>
+      </c>
+      <c r="D7">
+        <v>0.15329999999999999</v>
+      </c>
+      <c r="E7">
+        <v>-11.6812</v>
+      </c>
+      <c r="F7" s="3">
+        <v>514259.3125</v>
+      </c>
+      <c r="G7" s="40">
+        <v>297.97000000000003</v>
+      </c>
+      <c r="H7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7">
+        <v>1.4330000000000001</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1657.45</v>
+      </c>
+      <c r="K7" s="40">
+        <f>F7/B7</f>
+        <v>3254.8057753164558</v>
+      </c>
+      <c r="L7" s="3">
+        <f>(K7/G7)+(K7/E7)</f>
+        <v>-267.71298432259528</v>
+      </c>
+      <c r="M7" s="3">
+        <f>(K7/G7)+(K7/C7)</f>
+        <v>32.336462579223479</v>
+      </c>
+      <c r="N7" s="3">
+        <f>((K7/G7)+(K7/C7*B7))</f>
+        <v>3394.2082173468789</v>
+      </c>
+      <c r="P7" s="42">
+        <f t="shared" si="0"/>
+        <v>1.4898500000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="39">
+        <v>544</v>
+      </c>
+      <c r="C8" s="40">
         <v>112.35</v>
       </c>
-      <c r="D4">
-        <v>0.1118</v>
-      </c>
-      <c r="E4">
-        <v>-12.9529</v>
-      </c>
-      <c r="F4" s="3">
-        <v>706575.5</v>
-      </c>
-      <c r="G4" s="41">
-        <v>2004.55</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4">
-        <v>1.2081999999999999</v>
-      </c>
-      <c r="J4" s="3">
-        <v>5936.73</v>
-      </c>
-      <c r="K4" s="41">
-        <f>F4/B4</f>
-        <v>2379.0420875420878</v>
-      </c>
-      <c r="L4" s="3">
-        <f>+K4+C4+G4</f>
-        <v>4495.9420875420874</v>
-      </c>
-      <c r="N4" s="3"/>
+      <c r="D8">
+        <v>0.1172</v>
+      </c>
+      <c r="E8">
+        <v>-14.929500000000001</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1129507.5</v>
+      </c>
+      <c r="G8" s="40">
+        <v>165.79</v>
+      </c>
+      <c r="H8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8">
+        <v>1.4455</v>
+      </c>
+      <c r="J8" s="3">
+        <v>3240.82</v>
+      </c>
+      <c r="K8" s="40">
+        <f>F8/B8</f>
+        <v>2076.3005514705883</v>
+      </c>
+      <c r="L8" s="3">
+        <f>(K8/G8)+(K8/E8)</f>
+        <v>-126.55000522082177</v>
+      </c>
+      <c r="M8" s="3">
+        <f>(K8/G8)+(K8/C8)</f>
+        <v>31.004323617315436</v>
+      </c>
+      <c r="N8" s="3">
+        <f>((K8/G8)+(K8/C8*B8))</f>
+        <v>10065.994972914417</v>
+      </c>
+      <c r="P8" s="42">
+        <f t="shared" si="0"/>
+        <v>0.82894999999999996</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="40">
-        <v>427</v>
-      </c>
-      <c r="C5" s="41">
-        <v>129.19999999999999</v>
-      </c>
-      <c r="D5">
-        <v>0.1777</v>
-      </c>
-      <c r="E5">
-        <v>-11.209899999999999</v>
-      </c>
-      <c r="F5" s="3">
-        <v>1677930.375</v>
-      </c>
-      <c r="G5" s="41">
-        <v>294</v>
-      </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5">
-        <v>1.7843</v>
-      </c>
-      <c r="J5" s="3">
-        <v>7279.91</v>
-      </c>
-      <c r="K5" s="41">
-        <f>F5/B5</f>
-        <v>3929.5793325526934</v>
-      </c>
-      <c r="L5" s="3">
-        <f>+K5+C5+G5</f>
-        <v>4352.7793325526927</v>
-      </c>
-      <c r="N5" s="3"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="40">
-        <v>158</v>
-      </c>
-      <c r="C6" s="41">
-        <v>152</v>
-      </c>
-      <c r="D6">
-        <v>0.15329999999999999</v>
-      </c>
-      <c r="E6">
-        <v>-11.6812</v>
-      </c>
-      <c r="F6" s="3">
-        <v>514259.3125</v>
-      </c>
-      <c r="G6" s="41">
-        <v>297.97000000000003</v>
-      </c>
-      <c r="H6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6">
-        <v>1.4330000000000001</v>
-      </c>
-      <c r="J6" s="3">
-        <v>1657.45</v>
-      </c>
-      <c r="K6" s="41">
-        <f>F6/B6</f>
-        <v>3254.8057753164558</v>
-      </c>
-      <c r="L6" s="3">
-        <f>+K6+C6+G6</f>
-        <v>3704.775775316456</v>
-      </c>
-      <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="40">
-        <v>265</v>
-      </c>
-      <c r="C7" s="41">
-        <v>89.1</v>
-      </c>
-      <c r="D7">
-        <v>0.1426</v>
-      </c>
-      <c r="E7">
-        <v>-12.9703</v>
-      </c>
-      <c r="F7" s="3">
-        <v>756879.875</v>
-      </c>
-      <c r="G7" s="41">
-        <v>580.26</v>
-      </c>
-      <c r="H7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7">
-        <v>1.0942000000000001</v>
-      </c>
-      <c r="J7" s="3">
-        <v>7190.07</v>
-      </c>
-      <c r="K7" s="41">
-        <f>F7/B7</f>
-        <v>2856.1504716981131</v>
-      </c>
-      <c r="L7" s="3">
-        <f>+K7+C7+G7</f>
-        <v>3525.5104716981132</v>
-      </c>
-      <c r="N7" s="3"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="40">
-        <v>234</v>
-      </c>
-      <c r="C8" s="41">
-        <v>83.35</v>
-      </c>
-      <c r="D8">
-        <v>0.1225</v>
-      </c>
-      <c r="E8">
-        <v>-13.845499999999999</v>
-      </c>
-      <c r="F8" s="3">
-        <v>563190.75</v>
-      </c>
-      <c r="G8" s="41">
-        <v>648.53</v>
-      </c>
-      <c r="H8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8">
-        <v>1.5992</v>
-      </c>
-      <c r="J8" s="3">
-        <v>5888.17</v>
-      </c>
-      <c r="K8" s="41">
-        <f>F8/B8</f>
-        <v>2406.7980769230771</v>
-      </c>
-      <c r="L8" s="3">
-        <f>+K8+C8+G8</f>
-        <v>3138.6780769230772</v>
-      </c>
-      <c r="N8" s="3"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="40">
-        <v>158</v>
-      </c>
-      <c r="C9" s="41">
-        <v>129.19999999999999</v>
+        <v>29</v>
+      </c>
+      <c r="B9" s="39">
+        <v>104</v>
+      </c>
+      <c r="C9" s="40">
+        <v>92.29</v>
       </c>
       <c r="D9">
-        <v>0.1318</v>
+        <v>0.10249999999999999</v>
       </c>
       <c r="E9">
-        <v>-13.7721</v>
+        <v>-15.363200000000001</v>
       </c>
       <c r="F9" s="3">
-        <v>416358.8125</v>
-      </c>
-      <c r="G9" s="41">
-        <v>339.23</v>
+        <v>233933.890625</v>
+      </c>
+      <c r="G9" s="40">
+        <v>512.79</v>
       </c>
       <c r="H9" t="s">
         <v>30</v>
       </c>
       <c r="I9">
+        <v>1.1315999999999999</v>
+      </c>
+      <c r="J9" s="3">
+        <v>2078.71</v>
+      </c>
+      <c r="K9" s="40">
+        <f>F9/B9</f>
+        <v>2249.3643329326924</v>
+      </c>
+      <c r="L9" s="3">
+        <f>(K9/G9)+(K9/E9)</f>
+        <v>-142.02596637643069</v>
+      </c>
+      <c r="M9" s="3">
+        <f>(K9/G9)+(K9/C9)</f>
+        <v>28.759306504484996</v>
+      </c>
+      <c r="N9" s="3">
+        <f>((K9/G9)+(K9/C9*B9))</f>
+        <v>2539.1561674002191</v>
+      </c>
+      <c r="P9" s="42">
+        <f t="shared" si="0"/>
+        <v>2.5639499999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="39">
+        <v>158</v>
+      </c>
+      <c r="C10" s="40">
+        <v>129.19999999999999</v>
+      </c>
+      <c r="D10">
+        <v>0.1318</v>
+      </c>
+      <c r="E10">
+        <v>-13.7721</v>
+      </c>
+      <c r="F10" s="3">
+        <v>416358.8125</v>
+      </c>
+      <c r="G10" s="40">
+        <v>339.23</v>
+      </c>
+      <c r="H10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10">
         <v>1.1842999999999999</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J10" s="3">
         <v>1995.25</v>
       </c>
-      <c r="K9" s="41">
-        <f>F9/B9</f>
+      <c r="K10" s="40">
+        <f>F10/B10</f>
         <v>2635.1823575949365</v>
       </c>
-      <c r="L9" s="3">
-        <f>+K9+C9+G9</f>
-        <v>3103.6123575949364</v>
-      </c>
-      <c r="N9" s="3"/>
+      <c r="L10" s="3">
+        <f>(K10/G10)+(K10/E10)</f>
+        <v>-183.57395821572624</v>
+      </c>
+      <c r="M10" s="3">
+        <f>(K10/G10)+(K10/C10)</f>
+        <v>28.164277151619647</v>
+      </c>
+      <c r="N10" s="3">
+        <f>((K10/G10)+(K10/C10*B10))</f>
+        <v>3230.3595568915966</v>
+      </c>
+      <c r="P10" s="42">
+        <f t="shared" si="0"/>
+        <v>1.69615</v>
+      </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="40">
+      <c r="B11" s="39">
         <v>238</v>
       </c>
-      <c r="C10" s="41">
+      <c r="C11" s="40">
         <v>136</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <v>0.13439999999999999</v>
       </c>
-      <c r="E10">
+      <c r="E11">
         <v>-14.295199999999999</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F11" s="3">
         <v>603749.3125</v>
       </c>
-      <c r="G10" s="41">
+      <c r="G11" s="40">
         <v>408.33</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H11" t="s">
         <v>10</v>
       </c>
-      <c r="I10">
+      <c r="I11">
         <v>1.0834999999999999</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J11" s="3">
         <v>2960.79</v>
       </c>
-      <c r="K10" s="41">
-        <f>F10/B10</f>
+      <c r="K11" s="40">
+        <f>F11/B11</f>
         <v>2536.7618172268908</v>
       </c>
-      <c r="L10" s="3">
-        <f>+K10+C10+G10</f>
-        <v>3081.0918172268907</v>
-      </c>
-      <c r="N10" s="3"/>
+      <c r="L11" s="3">
+        <f>(K11/G11)+(K11/E11)</f>
+        <v>-171.24296812177758</v>
+      </c>
+      <c r="M11" s="3">
+        <f>(K11/G11)+(K11/C11)</f>
+        <v>24.865189055044752</v>
+      </c>
+      <c r="N11" s="3">
+        <f>((K11/G11)+(K11/C11*B11))</f>
+        <v>4445.5457087813184</v>
+      </c>
+      <c r="P11" s="42">
+        <f t="shared" si="0"/>
+        <v>2.0416499999999997</v>
+      </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="39">
+        <v>297</v>
+      </c>
+      <c r="C12" s="40">
+        <v>112.35</v>
+      </c>
+      <c r="D12">
+        <v>0.1118</v>
+      </c>
+      <c r="E12">
+        <v>-12.9529</v>
+      </c>
+      <c r="F12" s="3">
+        <v>706575.5</v>
+      </c>
+      <c r="G12" s="40">
+        <v>2004.55</v>
+      </c>
+      <c r="H12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12">
+        <v>1.2081999999999999</v>
+      </c>
+      <c r="J12" s="3">
+        <v>5936.73</v>
+      </c>
+      <c r="K12" s="40">
+        <f>F12/B12</f>
+        <v>2379.0420875420878</v>
+      </c>
+      <c r="L12" s="3">
+        <f>(K12/G12)+(K12/E12)</f>
+        <v>-182.48186224515189</v>
+      </c>
+      <c r="M12" s="3">
+        <f>(K12/G12)+(K12/C12)</f>
+        <v>22.362095503392201</v>
+      </c>
+      <c r="N12" s="3">
+        <f>((K12/G12)+(K12/C12*B12))</f>
+        <v>6290.2433408301213</v>
+      </c>
+      <c r="P12" s="42">
+        <f t="shared" si="0"/>
+        <v>10.02275</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="40">
+      <c r="B13" s="39">
         <v>232</v>
       </c>
-      <c r="C11" s="41">
+      <c r="C13" s="40">
         <v>161.5</v>
       </c>
-      <c r="D11">
+      <c r="D13">
         <v>0.12620000000000001</v>
       </c>
-      <c r="E11">
+      <c r="E13">
         <v>-13.6877</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F13" s="3">
         <v>504097.78125</v>
       </c>
-      <c r="G11" s="41">
+      <c r="G13" s="40">
         <v>551.25</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H13" t="s">
         <v>13</v>
       </c>
-      <c r="I11">
+      <c r="I13">
         <v>1.387</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J13" s="3">
         <v>2206.9</v>
       </c>
-      <c r="K11" s="41">
-        <f>F11/B11</f>
+      <c r="K13" s="40">
+        <f>F13/B13</f>
         <v>2172.8352640086205</v>
       </c>
-      <c r="L11" s="3">
-        <f>+K11+C11+G11</f>
-        <v>2885.5852640086205</v>
-      </c>
-      <c r="N11" s="3"/>
+      <c r="L13" s="3">
+        <f>(K13/G13)+(K13/E13)</f>
+        <v>-154.80198454707181</v>
+      </c>
+      <c r="M13" s="3">
+        <f>(K13/G13)+(K13/C13)</f>
+        <v>17.395739594612799</v>
+      </c>
+      <c r="N13" s="3">
+        <f>((K13/G13)+(K13/C13*B13))</f>
+        <v>3125.2901419846517</v>
+      </c>
+      <c r="P13" s="42">
+        <f t="shared" si="0"/>
+        <v>2.7562500000000001</v>
+      </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="40">
-        <v>104</v>
-      </c>
-      <c r="C12" s="41">
-        <v>92.29</v>
-      </c>
-      <c r="D12">
-        <v>0.10249999999999999</v>
-      </c>
-      <c r="E12">
-        <v>-15.363200000000001</v>
-      </c>
-      <c r="F12" s="3">
-        <v>233933.890625</v>
-      </c>
-      <c r="G12" s="41">
-        <v>512.79</v>
-      </c>
-      <c r="H12" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12">
-        <v>1.1315999999999999</v>
-      </c>
-      <c r="J12" s="3">
-        <v>2078.71</v>
-      </c>
-      <c r="K12" s="41">
-        <f>F12/B12</f>
-        <v>2249.3643329326924</v>
-      </c>
-      <c r="L12" s="3">
-        <f>+K12+C12+G12</f>
-        <v>2854.4443329326923</v>
-      </c>
-      <c r="N12" s="3"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="40">
-        <v>544</v>
-      </c>
-      <c r="C13" s="41">
-        <v>112.35</v>
-      </c>
-      <c r="D13">
-        <v>0.1172</v>
-      </c>
-      <c r="E13">
-        <v>-14.929500000000001</v>
-      </c>
-      <c r="F13" s="3">
-        <v>1129507.5</v>
-      </c>
-      <c r="G13" s="41">
-        <v>165.79</v>
-      </c>
-      <c r="H13" t="s">
-        <v>30</v>
-      </c>
-      <c r="I13">
-        <v>1.4455</v>
-      </c>
-      <c r="J13" s="3">
-        <v>3240.82</v>
-      </c>
-      <c r="K13" s="41">
-        <f>F13/B13</f>
-        <v>2076.3005514705883</v>
-      </c>
-      <c r="L13" s="3">
-        <f>+K13+C13+G13</f>
-        <v>2354.4405514705882</v>
-      </c>
-      <c r="N13" s="3"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="40">
-        <v>293</v>
+        <v>21</v>
+      </c>
+      <c r="B14" s="39">
+        <v>237</v>
       </c>
       <c r="C14" s="40">
-        <v>112.35</v>
+        <v>78.3</v>
       </c>
       <c r="D14">
-        <v>8.5000000000000006E-2</v>
+        <v>8.48E-2</v>
       </c>
       <c r="E14">
-        <v>-15.7897</v>
+        <v>-16.337700000000002</v>
       </c>
       <c r="F14" s="3">
-        <v>326635.5625</v>
+        <v>237987.46875</v>
       </c>
       <c r="G14" s="40">
-        <v>689.06</v>
+        <v>816.67</v>
       </c>
       <c r="H14" t="s">
         <v>19</v>
       </c>
       <c r="I14">
-        <v>0.93610000000000004</v>
-      </c>
-      <c r="J14">
-        <v>2433.35</v>
-      </c>
-      <c r="K14" s="41">
+        <v>1.1517999999999999</v>
+      </c>
+      <c r="J14" s="3">
+        <v>2747.92</v>
+      </c>
+      <c r="K14" s="40">
         <f>F14/B14</f>
-        <v>1114.7971416382252</v>
+        <v>1004.1665348101266</v>
       </c>
       <c r="L14" s="3">
-        <f>+K14+C14+G14</f>
-        <v>1916.207141638225</v>
-      </c>
-      <c r="N14" s="3"/>
+        <f>(K14/G14)+(K14/E14)</f>
+        <v>-60.233565121853182</v>
+      </c>
+      <c r="M14" s="3">
+        <f>(K14/G14)+(K14/C14)</f>
+        <v>14.054191187975901</v>
+      </c>
+      <c r="N14" s="3">
+        <f>((K14/G14)+(K14/C14*B14))</f>
+        <v>3040.6608606029172</v>
+      </c>
+      <c r="P14" s="42">
+        <f t="shared" si="0"/>
+        <v>4.0833499999999994</v>
+      </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="40">
-        <v>237</v>
-      </c>
-      <c r="C15" s="41">
-        <v>78.3</v>
+        <v>44</v>
+      </c>
+      <c r="B15" s="39">
+        <v>293</v>
+      </c>
+      <c r="C15" s="39">
+        <v>112.35</v>
       </c>
       <c r="D15">
-        <v>8.48E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="E15">
-        <v>-16.337700000000002</v>
+        <v>-15.7897</v>
       </c>
       <c r="F15" s="3">
-        <v>237987.46875</v>
-      </c>
-      <c r="G15" s="41">
-        <v>816.67</v>
+        <v>326635.5625</v>
+      </c>
+      <c r="G15" s="39">
+        <v>689.06</v>
       </c>
       <c r="H15" t="s">
         <v>19</v>
       </c>
       <c r="I15">
-        <v>1.1517999999999999</v>
-      </c>
-      <c r="J15" s="3">
-        <v>2747.92</v>
-      </c>
-      <c r="K15" s="41">
+        <v>0.93610000000000004</v>
+      </c>
+      <c r="J15">
+        <v>2433.35</v>
+      </c>
+      <c r="K15" s="40">
         <f>F15/B15</f>
-        <v>1004.1665348101266</v>
+        <v>1114.7971416382252</v>
       </c>
       <c r="L15" s="3">
-        <f>+K15+C15+G15</f>
-        <v>1899.1365348101267</v>
-      </c>
-      <c r="N15" s="3"/>
+        <f>(K15/G15)+(K15/E15)</f>
+        <v>-68.98495493514929</v>
+      </c>
+      <c r="M15" s="3">
+        <f>(K15/G15)+(K15/C15)</f>
+        <v>11.540390038012868</v>
+      </c>
+      <c r="N15" s="3">
+        <f>((K15/G15)+(K15/C15*B15))</f>
+        <v>2908.9214791200043</v>
+      </c>
+      <c r="P15" s="42">
+        <f t="shared" si="0"/>
+        <v>3.4452999999999996</v>
+      </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="40">
+      <c r="B16" s="39">
         <v>65</v>
       </c>
-      <c r="C16" s="41">
+      <c r="C16" s="40">
         <v>117.45</v>
       </c>
       <c r="D16">
@@ -1700,7 +1857,7 @@
       <c r="F16" s="3">
         <v>56900.1796875</v>
       </c>
-      <c r="G16" s="41">
+      <c r="G16" s="40">
         <v>250.57</v>
       </c>
       <c r="H16" t="s">
@@ -1712,24 +1869,35 @@
       <c r="J16" s="3">
         <v>257.36</v>
       </c>
-      <c r="K16" s="41">
+      <c r="K16" s="40">
         <f>F16/B16</f>
         <v>875.38737980769235</v>
       </c>
       <c r="L16" s="3">
-        <f>+K16+C16+G16</f>
-        <v>1243.4073798076925</v>
-      </c>
-      <c r="N16" s="3"/>
+        <f>(K16/G16)+(K16/E16)</f>
+        <v>-43.926413350374055</v>
+      </c>
+      <c r="M16" s="3">
+        <f>(K16/G16)+(K16/C16)</f>
+        <v>10.946861114660344</v>
+      </c>
+      <c r="N16" s="3">
+        <f>((K16/G16)+(K16/C16*B16))</f>
+        <v>487.956587020938</v>
+      </c>
+      <c r="P16" s="42">
+        <f t="shared" si="0"/>
+        <v>1.25285</v>
+      </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="40">
+      <c r="B17" s="39">
         <v>163</v>
       </c>
-      <c r="C17" s="41">
+      <c r="C17" s="40">
         <v>112.35</v>
       </c>
       <c r="D17">
@@ -1741,7 +1909,7 @@
       <c r="F17" s="3">
         <v>99084.421875</v>
       </c>
-      <c r="G17" s="41">
+      <c r="G17" s="40">
         <v>479.35</v>
       </c>
       <c r="H17" t="s">
@@ -1753,24 +1921,35 @@
       <c r="J17" s="3">
         <v>675.24</v>
       </c>
-      <c r="K17" s="41">
+      <c r="K17" s="40">
         <f>F17/B17</f>
         <v>607.87988880368096</v>
       </c>
       <c r="L17" s="3">
-        <f>+K17+C17+G17</f>
-        <v>1199.5798888036811</v>
-      </c>
-      <c r="N17" s="3"/>
+        <f>(K17/G17)+(K17/E17)</f>
+        <v>-31.390579185816595</v>
+      </c>
+      <c r="M17" s="3">
+        <f>(K17/G17)+(K17/C17)</f>
+        <v>6.6787246099724218</v>
+      </c>
+      <c r="N17" s="3">
+        <f>((K17/G17)+(K17/C17*B17))</f>
+        <v>883.19445212395829</v>
+      </c>
+      <c r="P17" s="42">
+        <f t="shared" si="0"/>
+        <v>2.3967499999999999</v>
+      </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="40">
+      <c r="B18" s="39">
         <v>284</v>
       </c>
-      <c r="C18" s="42">
+      <c r="C18" s="41">
         <v>129.19999999999999</v>
       </c>
       <c r="D18">
@@ -1782,7 +1961,7 @@
       <c r="F18" s="3">
         <v>143452.09375</v>
       </c>
-      <c r="G18" s="41">
+      <c r="G18" s="40">
         <v>512.79</v>
       </c>
       <c r="H18" t="s">
@@ -1794,24 +1973,35 @@
       <c r="J18" s="3">
         <v>830.57</v>
       </c>
-      <c r="K18" s="41">
+      <c r="K18" s="40">
         <f>F18/B18</f>
         <v>505.11300616197184</v>
       </c>
       <c r="L18" s="3">
-        <f>+K18+C18+G18</f>
-        <v>1147.1030061619717</v>
-      </c>
-      <c r="N18" s="3"/>
+        <f>(K18/G18)+(K18/E18)</f>
+        <v>-26.495888640466895</v>
+      </c>
+      <c r="M18" s="3">
+        <f>(K18/G18)+(K18/C18)</f>
+        <v>4.8945723625861657</v>
+      </c>
+      <c r="N18" s="3">
+        <f>((K18/G18)+(K18/C18*B18))</f>
+        <v>1111.2953521136546</v>
+      </c>
+      <c r="P18" s="42">
+        <f t="shared" si="0"/>
+        <v>2.5639499999999997</v>
+      </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="40">
+      <c r="B19" s="39">
         <v>273</v>
       </c>
-      <c r="C19" s="42">
+      <c r="C19" s="41">
         <v>152</v>
       </c>
       <c r="D19">
@@ -1823,7 +2013,7 @@
       <c r="F19" s="3">
         <v>114231.59375</v>
       </c>
-      <c r="G19" s="41">
+      <c r="G19" s="40">
         <v>256.39999999999998</v>
       </c>
       <c r="H19" t="s">
@@ -1835,24 +2025,34 @@
       <c r="J19" s="3">
         <v>306</v>
       </c>
-      <c r="K19" s="41">
+      <c r="K19" s="40">
         <f>F19/B19</f>
         <v>418.43074633699632</v>
       </c>
       <c r="L19" s="3">
-        <f>+K19+C19+G19</f>
-        <v>826.8307463369963</v>
-      </c>
-      <c r="M19" s="37"/>
-      <c r="N19" s="3"/>
+        <f>(K19/G19)+(K19/E19)</f>
+        <v>-18.39163468873252</v>
+      </c>
+      <c r="M19" s="3">
+        <f>(K19/G19)+(K19/C19)</f>
+        <v>4.3847790460020661</v>
+      </c>
+      <c r="N19" s="3">
+        <f>((K19/G19)+(K19/C19*B19))</f>
+        <v>753.15558828062717</v>
+      </c>
+      <c r="P19" s="42">
+        <f t="shared" si="0"/>
+        <v>1.2819999999999998</v>
+      </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="J23" s="16"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L19" xr:uid="{D881CB1C-05FC-3146-9C78-C0AA3598EAD0}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L19">
-      <sortCondition descending="1" ref="L1:L19"/>
+  <autoFilter ref="A1:N19" xr:uid="{D881CB1C-05FC-3146-9C78-C0AA3598EAD0}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N19">
+      <sortCondition descending="1" ref="M1:M19"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
aggiunta l'analisi in funzione del tempo, sembra funzionare il tutto - mette apposto il codice
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacopoazzetti/Documents/università/TESI/visual-audio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7F9E57-F9E6-2944-8423-F77A122BDF97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9B0505-4677-E344-87C5-E862D1620863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" xr2:uid="{539C8620-7C30-FF4C-9515-44D5778B2A1D}"/>
   </bookViews>
@@ -22,7 +22,7 @@
     <sheet name="Sorted by Pitch" sheetId="2" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'New Data'!$A$1:$N$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'New Data'!$B$1:$P$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="48">
   <si>
     <t>Song in Exam</t>
   </si>
@@ -187,6 +187,9 @@
   <si>
     <t>Time Energy</t>
   </si>
+  <si>
+    <t>Associated Color - Spectral Colormap</t>
+  </si>
 </sst>
 </file>
 
@@ -197,7 +200,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.00000000000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -234,8 +237,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="21">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -356,8 +375,104 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9F0042"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFECA78"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDFFBC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFECF8A3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD8EF9A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB8E3A1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9DD7A4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF86CEA4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66C2A6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF68C3A4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF58B4AA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4075B4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4969AE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF476CAF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF555AA7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -447,11 +562,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -536,7 +666,61 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -545,16 +729,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FF7FD76F"/>
-      <color rgb="FF55ED00"/>
-      <color rgb="FFF1F656"/>
-      <color rgb="FF299AFF"/>
-      <color rgb="FF8C6FFF"/>
-      <color rgb="FF2D87FF"/>
-      <color rgb="FF1FB9FF"/>
-      <color rgb="FF1BC6FF"/>
-      <color rgb="FF10E2F9"/>
-      <color rgb="FF46DAC5"/>
+      <color rgb="FF555AA7"/>
+      <color rgb="FF476CAF"/>
+      <color rgb="FF4969AE"/>
+      <color rgb="FF4075B4"/>
+      <color rgb="FF58B4AA"/>
+      <color rgb="FF68C3A4"/>
+      <color rgb="FF66C2A6"/>
+      <color rgb="FF86CEA4"/>
+      <color rgb="FF9DD7A4"/>
+      <color rgb="FFB8E3A1"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1052,1007 +1236,1085 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D881CB1C-05FC-3146-9C78-C0AA3598EAD0}">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="45"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="C1" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="D1" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="E1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="F1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="G1" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="H1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="I1" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="J1" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="K1" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="L1" s="37" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="47">
+        <v>14883.330931237137</v>
+      </c>
+      <c r="B2" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="39">
+      <c r="C2" s="39">
         <v>312</v>
       </c>
-      <c r="C2" s="40">
+      <c r="D2" s="40">
         <v>123.05</v>
       </c>
-      <c r="D2">
+      <c r="E2" s="42">
         <v>0.19470000000000001</v>
       </c>
-      <c r="E2">
+      <c r="F2" s="42">
         <v>-9.9871999999999996</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="43">
         <v>1831000.875</v>
       </c>
-      <c r="G2" s="40">
+      <c r="H2" s="40">
         <v>1837.5</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="I2">
+      <c r="J2" s="42">
         <v>1.3644000000000001</v>
       </c>
-      <c r="J2" s="3">
+      <c r="K2" s="43">
         <v>13884.05</v>
       </c>
-      <c r="K2" s="40">
-        <f>F2/B2</f>
+      <c r="L2" s="40">
+        <f>G2/C2</f>
         <v>5868.5925480769229</v>
       </c>
-      <c r="L2" s="3">
-        <f>(K2/G2)+(K2/E2)</f>
+      <c r="M2" s="3">
+        <f>(L2/H2)+(L2/F2)</f>
         <v>-584.41760553346057</v>
       </c>
-      <c r="M2" s="3">
-        <f>(K2/G2)+(K2/C2)</f>
-        <v>50.886539104483099</v>
-      </c>
       <c r="N2" s="3">
-        <f>((K2/G2)+(K2/C2*B2))</f>
+        <f>(L2/D2)-(L2/H2)</f>
+        <v>44.498955378685089</v>
+      </c>
+      <c r="O2" s="3">
+        <f>((L2/H2)+((L2/D2)*C2))</f>
         <v>14883.330931237137</v>
       </c>
-      <c r="P2" s="42">
-        <f>(G2)/200</f>
-        <v>9.1875</v>
-      </c>
+      <c r="P2" s="16">
+        <f>(L2*H2*(-F2))</f>
+        <v>107697358.77418269</v>
+      </c>
+      <c r="Q2" s="44"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" s="47">
+        <v>13000.443121979473</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="39">
+        <v>427</v>
+      </c>
+      <c r="D3" s="40">
+        <v>129.19999999999999</v>
+      </c>
+      <c r="E3">
+        <v>0.1777</v>
+      </c>
+      <c r="F3">
+        <v>-11.209899999999999</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1677930.375</v>
+      </c>
+      <c r="H3" s="40">
+        <v>294</v>
+      </c>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>1.7843</v>
+      </c>
+      <c r="K3" s="3">
+        <v>7279.91</v>
+      </c>
+      <c r="L3" s="40">
+        <f>G3/C3</f>
+        <v>3929.5793325526934</v>
+      </c>
+      <c r="M3" s="3">
+        <f>(L3/H3)+(L3/F3)</f>
+        <v>-337.17952432185928</v>
+      </c>
+      <c r="N3" s="3">
+        <f>(L3/D3)-(L3/H3)</f>
+        <v>17.048784619234112</v>
+      </c>
+      <c r="O3" s="3">
+        <f>((L3/H3)+((L3/D3)*C3))</f>
+        <v>13000.443121979473</v>
+      </c>
+      <c r="P3" s="16">
+        <f>(L3*H3*(-F3))</f>
+        <v>12950756.259834835</v>
+      </c>
+      <c r="Q3" s="44"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="47">
+        <v>10065.994972914417</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="39">
+        <v>544</v>
+      </c>
+      <c r="D4" s="40">
+        <v>112.35</v>
+      </c>
+      <c r="E4">
+        <v>0.1172</v>
+      </c>
+      <c r="F4">
+        <v>-14.929500000000001</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1129507.5</v>
+      </c>
+      <c r="H4" s="40">
+        <v>165.79</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4">
+        <v>1.4455</v>
+      </c>
+      <c r="K4" s="3">
+        <v>3240.82</v>
+      </c>
+      <c r="L4" s="40">
+        <f>G4/C4</f>
+        <v>2076.3005514705883</v>
+      </c>
+      <c r="M4" s="3">
+        <f>(L4/H4)+(L4/F4)</f>
+        <v>-126.55000522082177</v>
+      </c>
+      <c r="N4" s="3">
+        <f>(L4/D4)-(L4/H4)</f>
+        <v>5.9569679086407437</v>
+      </c>
+      <c r="O4" s="3">
+        <f>((L4/H4)+((L4/D4)*C4))</f>
+        <v>10065.994972914417</v>
+      </c>
+      <c r="P4" s="16">
+        <f>(L4*H4*(-F4))</f>
+        <v>5139179.8207004368</v>
+      </c>
+      <c r="Q4" s="44"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="48">
+        <v>8499.6458160059356</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="39">
+        <v>265</v>
+      </c>
+      <c r="D5" s="40">
+        <v>89.1</v>
+      </c>
+      <c r="E5">
+        <v>0.1426</v>
+      </c>
+      <c r="F5">
+        <v>-12.9703</v>
+      </c>
+      <c r="G5" s="3">
+        <v>756879.875</v>
+      </c>
+      <c r="H5" s="40">
+        <v>580.26</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5">
+        <v>1.0942000000000001</v>
+      </c>
+      <c r="K5" s="3">
+        <v>7190.07</v>
+      </c>
+      <c r="L5" s="40">
+        <f>G5/C5</f>
+        <v>2856.1504716981131</v>
+      </c>
+      <c r="M5" s="3">
+        <f>(L5/H5)+(L5/F5)</f>
+        <v>-215.28477980566842</v>
+      </c>
+      <c r="N5" s="3">
+        <f>(L5/D5)-(L5/H5)</f>
+        <v>27.133369983942828</v>
+      </c>
+      <c r="O5" s="3">
+        <f>((L5/H5)+((L5/D5)*C5))</f>
+        <v>8499.6458160059356</v>
+      </c>
+      <c r="P5" s="16">
+        <f>(L5*H5*(-F5))</f>
+        <v>21495806.241978697</v>
+      </c>
+      <c r="Q5" s="44"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="49">
+        <v>7498.7456442476796</v>
+      </c>
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="39">
+      <c r="C6" s="39">
         <v>190</v>
       </c>
-      <c r="C3" s="40">
+      <c r="D6" s="40">
         <v>123.05</v>
       </c>
-      <c r="D3">
+      <c r="E6">
         <v>0.18410000000000001</v>
       </c>
-      <c r="E3">
+      <c r="F6">
         <v>-10.3398</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G6" s="3">
         <v>921989.5</v>
       </c>
-      <c r="G3" s="40">
+      <c r="H6" s="40">
         <v>816.67</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I6" t="s">
         <v>10</v>
       </c>
-      <c r="I3">
+      <c r="J6">
         <v>1.1934</v>
       </c>
-      <c r="J3" s="3">
-        <f>+(F3/C3)-(F3/G3)</f>
+      <c r="K6" s="3">
+        <f>+(G6/D6)-(G6/H6)</f>
         <v>6363.8416116325598</v>
       </c>
-      <c r="K3" s="40">
-        <f>F3/B3</f>
+      <c r="L6" s="40">
+        <f>G6/C6</f>
         <v>4852.5763157894735</v>
       </c>
-      <c r="L3" s="3">
-        <f>(K3/G3)+(K3/E3)</f>
+      <c r="M6" s="3">
+        <f>(L6/H6)+(L6/F6)</f>
         <v>-463.36855614763004</v>
       </c>
-      <c r="M3" s="3">
-        <f>(K3/G3)+(K3/C3)</f>
-        <v>45.377715078962922</v>
-      </c>
-      <c r="N3" s="3">
-        <f>((K3/G3)+(K3/C3*B3))</f>
+      <c r="N6" s="3">
+        <f>(L6/D6)-(L6/H6)</f>
+        <v>33.493903219118735</v>
+      </c>
+      <c r="O6" s="3">
+        <f>((L6/H6)+((L6/D6)*C6))</f>
         <v>7498.7456442476796</v>
       </c>
-      <c r="P3" s="42">
-        <f t="shared" ref="P3:P19" si="0">(G3)/200</f>
-        <v>4.0833499999999994</v>
-      </c>
+      <c r="P6" s="16">
+        <f>(L6*H6*(-F6))</f>
+        <v>40976146.597395293</v>
+      </c>
+      <c r="Q6" s="44"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="39">
-        <v>427</v>
-      </c>
-      <c r="C4" s="40">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="50">
+        <v>6760.6487716789661</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="39">
+        <v>234</v>
+      </c>
+      <c r="D7" s="40">
+        <v>83.35</v>
+      </c>
+      <c r="E7">
+        <v>0.1225</v>
+      </c>
+      <c r="F7">
+        <v>-13.845499999999999</v>
+      </c>
+      <c r="G7" s="3">
+        <v>563190.75</v>
+      </c>
+      <c r="H7" s="40">
+        <v>648.53</v>
+      </c>
+      <c r="I7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7">
+        <v>1.5992</v>
+      </c>
+      <c r="K7" s="3">
+        <v>5888.17</v>
+      </c>
+      <c r="L7" s="40">
+        <f>G7/C7</f>
+        <v>2406.7980769230771</v>
+      </c>
+      <c r="M7" s="3">
+        <f>(L7/H7)+(L7/F7)</f>
+        <v>-170.12135511171559</v>
+      </c>
+      <c r="N7" s="3">
+        <f>(L7/D7)-(L7/H7)</f>
+        <v>25.164642561264039</v>
+      </c>
+      <c r="O7" s="3">
+        <f>((L7/H7)+((L7/D7)*C7))</f>
+        <v>6760.6487716789661</v>
+      </c>
+      <c r="P7" s="16">
+        <f>(L7*H7*(-F7))</f>
+        <v>21611174.518647164</v>
+      </c>
+      <c r="Q7" s="44"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="51">
+        <v>6290.2433408301213</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="39">
+        <v>297</v>
+      </c>
+      <c r="D8" s="40">
+        <v>112.35</v>
+      </c>
+      <c r="E8">
+        <v>0.1118</v>
+      </c>
+      <c r="F8">
+        <v>-12.9529</v>
+      </c>
+      <c r="G8" s="3">
+        <v>706575.5</v>
+      </c>
+      <c r="H8" s="40">
+        <v>2004.55</v>
+      </c>
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8">
+        <v>1.2081999999999999</v>
+      </c>
+      <c r="K8" s="3">
+        <v>5936.73</v>
+      </c>
+      <c r="L8" s="40">
+        <f>G8/C8</f>
+        <v>2379.0420875420878</v>
+      </c>
+      <c r="M8" s="3">
+        <f>(L8/H8)+(L8/F8)</f>
+        <v>-182.48186224515189</v>
+      </c>
+      <c r="N8" s="3">
+        <f>(L8/D8)-(L8/H8)</f>
+        <v>19.988453451518129</v>
+      </c>
+      <c r="O8" s="3">
+        <f>((L8/H8)+((L8/D8)*C8))</f>
+        <v>6290.2433408301213</v>
+      </c>
+      <c r="P8" s="16">
+        <f>(L8*H8*(-F8))</f>
+        <v>61771199.010311358</v>
+      </c>
+      <c r="Q8" s="44"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="52">
+        <v>4445.5457087813184</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="39">
+        <v>238</v>
+      </c>
+      <c r="D9" s="40">
+        <v>136</v>
+      </c>
+      <c r="E9">
+        <v>0.13439999999999999</v>
+      </c>
+      <c r="F9">
+        <v>-14.295199999999999</v>
+      </c>
+      <c r="G9" s="3">
+        <v>603749.3125</v>
+      </c>
+      <c r="H9" s="40">
+        <v>408.33</v>
+      </c>
+      <c r="I9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9">
+        <v>1.0834999999999999</v>
+      </c>
+      <c r="K9" s="3">
+        <v>2960.79</v>
+      </c>
+      <c r="L9" s="40">
+        <f>G9/C9</f>
+        <v>2536.7618172268908</v>
+      </c>
+      <c r="M9" s="3">
+        <f>(L9/H9)+(L9/F9)</f>
+        <v>-171.24296812177758</v>
+      </c>
+      <c r="N9" s="3">
+        <f>(L9/D9)-(L9/H9)</f>
+        <v>12.440131786527175</v>
+      </c>
+      <c r="O9" s="3">
+        <f>((L9/H9)+((L9/D9)*C9))</f>
+        <v>4445.5457087813184</v>
+      </c>
+      <c r="P9" s="16">
+        <f>(L9*H9*(-F9))</f>
+        <v>14807482.112870488</v>
+      </c>
+      <c r="Q9" s="44"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="53">
+        <v>3394.2082173468789</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="39">
+        <v>158</v>
+      </c>
+      <c r="D10" s="40">
+        <v>152</v>
+      </c>
+      <c r="E10">
+        <v>0.15329999999999999</v>
+      </c>
+      <c r="F10">
+        <v>-11.6812</v>
+      </c>
+      <c r="G10" s="3">
+        <v>514259.3125</v>
+      </c>
+      <c r="H10" s="40">
+        <v>297.97000000000003</v>
+      </c>
+      <c r="I10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10">
+        <v>1.4330000000000001</v>
+      </c>
+      <c r="K10" s="3">
+        <v>1657.45</v>
+      </c>
+      <c r="L10" s="40">
+        <f>G10/C10</f>
+        <v>3254.8057753164558</v>
+      </c>
+      <c r="M10" s="3">
+        <f>(L10/H10)+(L10/F10)</f>
+        <v>-267.71298432259528</v>
+      </c>
+      <c r="N10" s="3">
+        <f>(L10/D10)-(L10/H10)</f>
+        <v>10.489929201256199</v>
+      </c>
+      <c r="O10" s="3">
+        <f>((L10/H10)+((L10/D10)*C10))</f>
+        <v>3394.2082173468789</v>
+      </c>
+      <c r="P10" s="16">
+        <f>(L10*H10*(-F10))</f>
+        <v>11328830.491226044</v>
+      </c>
+      <c r="Q10" s="44"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="54">
+        <v>3230.3595568915966</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="39">
+        <v>158</v>
+      </c>
+      <c r="D11" s="40">
         <v>129.19999999999999</v>
       </c>
-      <c r="D4">
-        <v>0.1777</v>
-      </c>
-      <c r="E4">
-        <v>-11.209899999999999</v>
-      </c>
-      <c r="F4" s="3">
-        <v>1677930.375</v>
-      </c>
-      <c r="G4" s="40">
-        <v>294</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4">
-        <v>1.7843</v>
-      </c>
-      <c r="J4" s="3">
-        <v>7279.91</v>
-      </c>
-      <c r="K4" s="40">
-        <f>F4/B4</f>
-        <v>3929.5793325526934</v>
-      </c>
-      <c r="L4" s="3">
-        <f>(K4/G4)+(K4/E4)</f>
-        <v>-337.17952432185928</v>
-      </c>
-      <c r="M4" s="3">
-        <f>(K4/G4)+(K4/C4)</f>
-        <v>43.780616813470125</v>
-      </c>
-      <c r="N4" s="3">
-        <f>((K4/G4)+(K4/C4*B4))</f>
-        <v>13000.443121979473</v>
-      </c>
-      <c r="P4" s="42">
-        <f t="shared" si="0"/>
-        <v>1.47</v>
-      </c>
+      <c r="E11">
+        <v>0.1318</v>
+      </c>
+      <c r="F11">
+        <v>-13.7721</v>
+      </c>
+      <c r="G11" s="3">
+        <v>416358.8125</v>
+      </c>
+      <c r="H11" s="40">
+        <v>339.23</v>
+      </c>
+      <c r="I11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11">
+        <v>1.1842999999999999</v>
+      </c>
+      <c r="K11" s="3">
+        <v>1995.25</v>
+      </c>
+      <c r="L11" s="40">
+        <f>G11/C11</f>
+        <v>2635.1823575949365</v>
+      </c>
+      <c r="M11" s="3">
+        <f>(L11/H11)+(L11/F11)</f>
+        <v>-183.57395821572624</v>
+      </c>
+      <c r="N11" s="3">
+        <f>(L11/D11)-(L11/H11)</f>
+        <v>12.628019405577515</v>
+      </c>
+      <c r="O11" s="3">
+        <f>((L11/H11)+((L11/D11)*C11))</f>
+        <v>3230.3595568915966</v>
+      </c>
+      <c r="P11" s="16">
+        <f>(L11*H11*(-F11))</f>
+        <v>12311333.445882082</v>
+      </c>
+      <c r="Q11" s="44"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="39">
-        <v>265</v>
-      </c>
-      <c r="C5" s="40">
-        <v>89.1</v>
-      </c>
-      <c r="D5">
-        <v>0.1426</v>
-      </c>
-      <c r="E5">
-        <v>-12.9703</v>
-      </c>
-      <c r="F5" s="3">
-        <v>756879.875</v>
-      </c>
-      <c r="G5" s="40">
-        <v>580.26</v>
-      </c>
-      <c r="H5" t="s">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="55">
+        <v>3125.2901419846517</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="39">
+        <v>232</v>
+      </c>
+      <c r="D12" s="40">
+        <v>161.5</v>
+      </c>
+      <c r="E12">
+        <v>0.12620000000000001</v>
+      </c>
+      <c r="F12">
+        <v>-13.6877</v>
+      </c>
+      <c r="G12" s="3">
+        <v>504097.78125</v>
+      </c>
+      <c r="H12" s="40">
+        <v>551.25</v>
+      </c>
+      <c r="I12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12">
+        <v>1.387</v>
+      </c>
+      <c r="K12" s="3">
+        <v>2206.9</v>
+      </c>
+      <c r="L12" s="40">
+        <f>G12/C12</f>
+        <v>2172.8352640086205</v>
+      </c>
+      <c r="M12" s="3">
+        <f>(L12/H12)+(L12/F12)</f>
+        <v>-154.80198454707181</v>
+      </c>
+      <c r="N12" s="3">
+        <f>(L12/D12)-(L12/H12)</f>
+        <v>9.5124370494568051</v>
+      </c>
+      <c r="O12" s="3">
+        <f>((L12/H12)+((L12/D12)*C12))</f>
+        <v>3125.2901419846517</v>
+      </c>
+      <c r="P12" s="16">
+        <f>(L12*H12*(-F12))</f>
+        <v>16394790.880297901</v>
+      </c>
+      <c r="Q12" s="44"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="56">
+        <v>3040.6608606029172</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="39">
+        <v>237</v>
+      </c>
+      <c r="D13" s="40">
+        <v>78.3</v>
+      </c>
+      <c r="E13">
+        <v>8.48E-2</v>
+      </c>
+      <c r="F13">
+        <v>-16.337700000000002</v>
+      </c>
+      <c r="G13" s="3">
+        <v>237987.46875</v>
+      </c>
+      <c r="H13" s="40">
+        <v>816.67</v>
+      </c>
+      <c r="I13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13">
+        <v>1.1517999999999999</v>
+      </c>
+      <c r="K13" s="3">
+        <v>2747.92</v>
+      </c>
+      <c r="L13" s="40">
+        <f>G13/C13</f>
+        <v>1004.1665348101266</v>
+      </c>
+      <c r="M13" s="3">
+        <f>(L13/H13)+(L13/F13)</f>
+        <v>-60.233565121853182</v>
+      </c>
+      <c r="N13" s="3">
+        <f>(L13/D13)-(L13/H13)</f>
+        <v>11.595017874862583</v>
+      </c>
+      <c r="O13" s="3">
+        <f>((L13/H13)+((L13/D13)*C13))</f>
+        <v>3040.6608606029172</v>
+      </c>
+      <c r="P13" s="16">
+        <f>(L13*H13*(-F13))</f>
+        <v>13398101.489115367</v>
+      </c>
+      <c r="Q13" s="44"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="57">
+        <v>2908.9214791200043</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="39">
+        <v>293</v>
+      </c>
+      <c r="D14" s="39">
+        <v>112.35</v>
+      </c>
+      <c r="E14">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="F14">
+        <v>-15.7897</v>
+      </c>
+      <c r="G14" s="3">
+        <v>326635.5625</v>
+      </c>
+      <c r="H14" s="39">
+        <v>689.06</v>
+      </c>
+      <c r="I14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14">
+        <v>0.93610000000000004</v>
+      </c>
+      <c r="K14">
+        <v>2433.35</v>
+      </c>
+      <c r="L14" s="40">
+        <f>G14/C14</f>
+        <v>1114.7971416382252</v>
+      </c>
+      <c r="M14" s="3">
+        <f>(L14/H14)+(L14/F14)</f>
+        <v>-68.98495493514929</v>
+      </c>
+      <c r="N14" s="3">
+        <f>(L14/D14)-(L14/H14)</f>
+        <v>8.3046859146035121</v>
+      </c>
+      <c r="O14" s="3">
+        <f>((L14/H14)+((L14/D14)*C14))</f>
+        <v>2908.9214791200043</v>
+      </c>
+      <c r="P14" s="16">
+        <f>(L14*H14*(-F14))</f>
+        <v>12129049.401172623</v>
+      </c>
+      <c r="Q14" s="44"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="58">
+        <v>2539.1561674002191</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="39">
+        <v>104</v>
+      </c>
+      <c r="D15" s="40">
+        <v>92.29</v>
+      </c>
+      <c r="E15">
+        <v>0.10249999999999999</v>
+      </c>
+      <c r="F15">
+        <v>-15.363200000000001</v>
+      </c>
+      <c r="G15" s="3">
+        <v>233933.890625</v>
+      </c>
+      <c r="H15" s="40">
+        <v>512.79</v>
+      </c>
+      <c r="I15" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15">
+        <v>1.1315999999999999</v>
+      </c>
+      <c r="K15" s="3">
+        <v>2078.71</v>
+      </c>
+      <c r="L15" s="40">
+        <f>G15/C15</f>
+        <v>2249.3643329326924</v>
+      </c>
+      <c r="M15" s="3">
+        <f>(L15/H15)+(L15/F15)</f>
+        <v>-142.02596637643069</v>
+      </c>
+      <c r="N15" s="3">
+        <f>(L15/D15)-(L15/H15)</f>
+        <v>19.986263609995277</v>
+      </c>
+      <c r="O15" s="3">
+        <f>((L15/H15)+((L15/D15)*C15))</f>
+        <v>2539.1561674002191</v>
+      </c>
+      <c r="P15" s="16">
+        <f>(L15*H15*(-F15))</f>
+        <v>17720706.64224688</v>
+      </c>
+      <c r="Q15" s="44"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="59">
+        <v>1111.2953521136546</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="39">
+        <v>284</v>
+      </c>
+      <c r="D16" s="41">
+        <v>129.19999999999999</v>
+      </c>
+      <c r="E16">
+        <v>5.2299999999999999E-2</v>
+      </c>
+      <c r="F16">
+        <v>-18.380500000000001</v>
+      </c>
+      <c r="G16" s="3">
+        <v>143452.09375</v>
+      </c>
+      <c r="H16" s="40">
+        <v>512.79</v>
+      </c>
+      <c r="I16" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16">
+        <v>0.98119999999999996</v>
+      </c>
+      <c r="K16" s="3">
+        <v>830.57</v>
+      </c>
+      <c r="L16" s="40">
+        <f>G16/C16</f>
+        <v>505.11300616197184</v>
+      </c>
+      <c r="M16" s="3">
+        <f>(L16/H16)+(L16/F16)</f>
+        <v>-26.495888640466895</v>
+      </c>
+      <c r="N16" s="3">
+        <f>(L16/D16)-(L16/H16)</f>
+        <v>2.9245144201068975</v>
+      </c>
+      <c r="O16" s="3">
+        <f>((L16/H16)+((L16/D16)*C16))</f>
+        <v>1111.2953521136546</v>
+      </c>
+      <c r="P16" s="16">
+        <f>(L16*H16*(-F16))</f>
+        <v>4760860.1015888937</v>
+      </c>
+      <c r="Q16" s="44"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" s="60">
+        <v>883.19445212395829</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="39">
+        <v>163</v>
+      </c>
+      <c r="D17" s="40">
+        <v>112.35</v>
+      </c>
+      <c r="E17">
+        <v>6.5699999999999995E-2</v>
+      </c>
+      <c r="F17">
+        <v>-18.613099999999999</v>
+      </c>
+      <c r="G17" s="3">
+        <v>99084.421875</v>
+      </c>
+      <c r="H17" s="40">
+        <v>479.35</v>
+      </c>
+      <c r="I17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17">
+        <v>1.0147999999999999</v>
+      </c>
+      <c r="K17" s="3">
+        <v>675.24</v>
+      </c>
+      <c r="L17" s="40">
+        <f>G17/C17</f>
+        <v>607.87988880368096</v>
+      </c>
+      <c r="M17" s="3">
+        <f>(L17/H17)+(L17/F17)</f>
+        <v>-31.390579185816595</v>
+      </c>
+      <c r="N17" s="3">
+        <f>(L17/D17)-(L17/H17)</f>
+        <v>4.1424572111878977</v>
+      </c>
+      <c r="O17" s="3">
+        <f>((L17/H17)+((L17/D17)*C17))</f>
+        <v>883.19445212395829</v>
+      </c>
+      <c r="P17" s="16">
+        <f>(L17*H17*(-F17))</f>
+        <v>5423619.5520271715</v>
+      </c>
+      <c r="Q17" s="44"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18" s="61">
+        <v>753.15558828062717</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="39">
+        <v>273</v>
+      </c>
+      <c r="D18" s="41">
+        <v>152</v>
+      </c>
+      <c r="E18">
+        <v>4.7800000000000002E-2</v>
+      </c>
+      <c r="F18">
+        <v>-20.896899999999999</v>
+      </c>
+      <c r="G18" s="3">
+        <v>114231.59375</v>
+      </c>
+      <c r="H18" s="40">
+        <v>256.39999999999998</v>
+      </c>
+      <c r="I18" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18">
+        <v>1.2103999999999999</v>
+      </c>
+      <c r="K18" s="3">
+        <v>306</v>
+      </c>
+      <c r="L18" s="40">
+        <f>G18/C18</f>
+        <v>418.43074633699632</v>
+      </c>
+      <c r="M18" s="3">
+        <f>(L18/H18)+(L18/F18)</f>
+        <v>-18.39163468873252</v>
+      </c>
+      <c r="N18" s="3">
+        <f>(L18/D18)-(L18/H18)</f>
+        <v>1.1208886689584125</v>
+      </c>
+      <c r="O18" s="3">
+        <f>((L18/H18)+((L18/D18)*C18))</f>
+        <v>753.15558828062717</v>
+      </c>
+      <c r="P18" s="16">
+        <f>(L18*H18*(-F18))</f>
+        <v>2241937.3607464237</v>
+      </c>
+      <c r="Q18" s="44"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19" s="62">
+        <v>487.956587020938</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="39">
+        <v>65</v>
+      </c>
+      <c r="D19" s="40">
+        <v>117.45</v>
+      </c>
+      <c r="E19">
+        <v>7.6600000000000001E-2</v>
+      </c>
+      <c r="F19">
+        <v>-18.4603</v>
+      </c>
+      <c r="G19" s="3">
+        <v>56900.1796875</v>
+      </c>
+      <c r="H19" s="40">
+        <v>250.57</v>
+      </c>
+      <c r="I19" t="s">
         <v>18</v>
       </c>
-      <c r="I5">
-        <v>1.0942000000000001</v>
-      </c>
-      <c r="J5" s="3">
-        <v>7190.07</v>
-      </c>
-      <c r="K5" s="40">
-        <f>F5/B5</f>
-        <v>2856.1504716981131</v>
-      </c>
-      <c r="L5" s="3">
-        <f>(K5/G5)+(K5/E5)</f>
-        <v>-215.28477980566842</v>
-      </c>
-      <c r="M5" s="3">
-        <f>(K5/G5)+(K5/C5)</f>
-        <v>36.977751715229189</v>
-      </c>
-      <c r="N5" s="3">
-        <f>((K5/G5)+(K5/C5*B5))</f>
-        <v>8499.6458160059356</v>
-      </c>
-      <c r="P5" s="42">
-        <f t="shared" si="0"/>
-        <v>2.9013</v>
-      </c>
+      <c r="J19">
+        <v>0.872</v>
+      </c>
+      <c r="K19" s="3">
+        <v>257.36</v>
+      </c>
+      <c r="L19" s="40">
+        <f>G19/C19</f>
+        <v>875.38737980769235</v>
+      </c>
+      <c r="M19" s="3">
+        <f>(L19/H19)+(L19/F19)</f>
+        <v>-43.926413350374055</v>
+      </c>
+      <c r="N19" s="3">
+        <f>(L19/D19)-(L19/H19)</f>
+        <v>3.9596928199108334</v>
+      </c>
+      <c r="O19" s="3">
+        <f>((L19/H19)+((L19/D19)*C19))</f>
+        <v>487.956587020938</v>
+      </c>
+      <c r="P19" s="16">
+        <f>(L19*H19*(-F19))</f>
+        <v>4049189.56264504</v>
+      </c>
+      <c r="Q19" s="44"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="39">
-        <v>234</v>
-      </c>
-      <c r="C6" s="40">
-        <v>83.35</v>
-      </c>
-      <c r="D6">
-        <v>0.1225</v>
-      </c>
-      <c r="E6">
-        <v>-13.845499999999999</v>
-      </c>
-      <c r="F6" s="3">
-        <v>563190.75</v>
-      </c>
-      <c r="G6" s="40">
-        <v>648.53</v>
-      </c>
-      <c r="H6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6">
-        <v>1.5992</v>
-      </c>
-      <c r="J6" s="3">
-        <v>5888.17</v>
-      </c>
-      <c r="K6" s="40">
-        <f>F6/B6</f>
-        <v>2406.7980769230771</v>
-      </c>
-      <c r="L6" s="3">
-        <f>(K6/G6)+(K6/E6)</f>
-        <v>-170.12135511171559</v>
-      </c>
-      <c r="M6" s="3">
-        <f>(K6/G6)+(K6/C6)</f>
-        <v>32.586960964184726</v>
-      </c>
-      <c r="N6" s="3">
-        <f>((K6/G6)+(K6/C6*B6))</f>
-        <v>6760.6487716789661</v>
-      </c>
-      <c r="P6" s="42">
-        <f t="shared" si="0"/>
-        <v>3.2426499999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="39">
-        <v>158</v>
-      </c>
-      <c r="C7" s="40">
-        <v>152</v>
-      </c>
-      <c r="D7">
-        <v>0.15329999999999999</v>
-      </c>
-      <c r="E7">
-        <v>-11.6812</v>
-      </c>
-      <c r="F7" s="3">
-        <v>514259.3125</v>
-      </c>
-      <c r="G7" s="40">
-        <v>297.97000000000003</v>
-      </c>
-      <c r="H7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7">
-        <v>1.4330000000000001</v>
-      </c>
-      <c r="J7" s="3">
-        <v>1657.45</v>
-      </c>
-      <c r="K7" s="40">
-        <f>F7/B7</f>
-        <v>3254.8057753164558</v>
-      </c>
-      <c r="L7" s="3">
-        <f>(K7/G7)+(K7/E7)</f>
-        <v>-267.71298432259528</v>
-      </c>
-      <c r="M7" s="3">
-        <f>(K7/G7)+(K7/C7)</f>
-        <v>32.336462579223479</v>
-      </c>
-      <c r="N7" s="3">
-        <f>((K7/G7)+(K7/C7*B7))</f>
-        <v>3394.2082173468789</v>
-      </c>
-      <c r="P7" s="42">
-        <f t="shared" si="0"/>
-        <v>1.4898500000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="39">
-        <v>544</v>
-      </c>
-      <c r="C8" s="40">
-        <v>112.35</v>
-      </c>
-      <c r="D8">
-        <v>0.1172</v>
-      </c>
-      <c r="E8">
-        <v>-14.929500000000001</v>
-      </c>
-      <c r="F8" s="3">
-        <v>1129507.5</v>
-      </c>
-      <c r="G8" s="40">
-        <v>165.79</v>
-      </c>
-      <c r="H8" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8">
-        <v>1.4455</v>
-      </c>
-      <c r="J8" s="3">
-        <v>3240.82</v>
-      </c>
-      <c r="K8" s="40">
-        <f>F8/B8</f>
-        <v>2076.3005514705883</v>
-      </c>
-      <c r="L8" s="3">
-        <f>(K8/G8)+(K8/E8)</f>
-        <v>-126.55000522082177</v>
-      </c>
-      <c r="M8" s="3">
-        <f>(K8/G8)+(K8/C8)</f>
-        <v>31.004323617315436</v>
-      </c>
-      <c r="N8" s="3">
-        <f>((K8/G8)+(K8/C8*B8))</f>
-        <v>10065.994972914417</v>
-      </c>
-      <c r="P8" s="42">
-        <f t="shared" si="0"/>
-        <v>0.82894999999999996</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="39">
-        <v>104</v>
-      </c>
-      <c r="C9" s="40">
-        <v>92.29</v>
-      </c>
-      <c r="D9">
-        <v>0.10249999999999999</v>
-      </c>
-      <c r="E9">
-        <v>-15.363200000000001</v>
-      </c>
-      <c r="F9" s="3">
-        <v>233933.890625</v>
-      </c>
-      <c r="G9" s="40">
-        <v>512.79</v>
-      </c>
-      <c r="H9" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9">
-        <v>1.1315999999999999</v>
-      </c>
-      <c r="J9" s="3">
-        <v>2078.71</v>
-      </c>
-      <c r="K9" s="40">
-        <f>F9/B9</f>
-        <v>2249.3643329326924</v>
-      </c>
-      <c r="L9" s="3">
-        <f>(K9/G9)+(K9/E9)</f>
-        <v>-142.02596637643069</v>
-      </c>
-      <c r="M9" s="3">
-        <f>(K9/G9)+(K9/C9)</f>
-        <v>28.759306504484996</v>
-      </c>
-      <c r="N9" s="3">
-        <f>((K9/G9)+(K9/C9*B9))</f>
-        <v>2539.1561674002191</v>
-      </c>
-      <c r="P9" s="42">
-        <f t="shared" si="0"/>
-        <v>2.5639499999999997</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="39">
-        <v>158</v>
-      </c>
-      <c r="C10" s="40">
-        <v>129.19999999999999</v>
-      </c>
-      <c r="D10">
-        <v>0.1318</v>
-      </c>
-      <c r="E10">
-        <v>-13.7721</v>
-      </c>
-      <c r="F10" s="3">
-        <v>416358.8125</v>
-      </c>
-      <c r="G10" s="40">
-        <v>339.23</v>
-      </c>
-      <c r="H10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10">
-        <v>1.1842999999999999</v>
-      </c>
-      <c r="J10" s="3">
-        <v>1995.25</v>
-      </c>
-      <c r="K10" s="40">
-        <f>F10/B10</f>
-        <v>2635.1823575949365</v>
-      </c>
-      <c r="L10" s="3">
-        <f>(K10/G10)+(K10/E10)</f>
-        <v>-183.57395821572624</v>
-      </c>
-      <c r="M10" s="3">
-        <f>(K10/G10)+(K10/C10)</f>
-        <v>28.164277151619647</v>
-      </c>
-      <c r="N10" s="3">
-        <f>((K10/G10)+(K10/C10*B10))</f>
-        <v>3230.3595568915966</v>
-      </c>
-      <c r="P10" s="42">
-        <f t="shared" si="0"/>
-        <v>1.69615</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="39">
-        <v>238</v>
-      </c>
-      <c r="C11" s="40">
-        <v>136</v>
-      </c>
-      <c r="D11">
-        <v>0.13439999999999999</v>
-      </c>
-      <c r="E11">
-        <v>-14.295199999999999</v>
-      </c>
-      <c r="F11" s="3">
-        <v>603749.3125</v>
-      </c>
-      <c r="G11" s="40">
-        <v>408.33</v>
-      </c>
-      <c r="H11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11">
-        <v>1.0834999999999999</v>
-      </c>
-      <c r="J11" s="3">
-        <v>2960.79</v>
-      </c>
-      <c r="K11" s="40">
-        <f>F11/B11</f>
-        <v>2536.7618172268908</v>
-      </c>
-      <c r="L11" s="3">
-        <f>(K11/G11)+(K11/E11)</f>
-        <v>-171.24296812177758</v>
-      </c>
-      <c r="M11" s="3">
-        <f>(K11/G11)+(K11/C11)</f>
-        <v>24.865189055044752</v>
-      </c>
-      <c r="N11" s="3">
-        <f>((K11/G11)+(K11/C11*B11))</f>
-        <v>4445.5457087813184</v>
-      </c>
-      <c r="P11" s="42">
-        <f t="shared" si="0"/>
-        <v>2.0416499999999997</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="39">
-        <v>297</v>
-      </c>
-      <c r="C12" s="40">
-        <v>112.35</v>
-      </c>
-      <c r="D12">
-        <v>0.1118</v>
-      </c>
-      <c r="E12">
-        <v>-12.9529</v>
-      </c>
-      <c r="F12" s="3">
-        <v>706575.5</v>
-      </c>
-      <c r="G12" s="40">
-        <v>2004.55</v>
-      </c>
-      <c r="H12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12">
-        <v>1.2081999999999999</v>
-      </c>
-      <c r="J12" s="3">
-        <v>5936.73</v>
-      </c>
-      <c r="K12" s="40">
-        <f>F12/B12</f>
-        <v>2379.0420875420878</v>
-      </c>
-      <c r="L12" s="3">
-        <f>(K12/G12)+(K12/E12)</f>
-        <v>-182.48186224515189</v>
-      </c>
-      <c r="M12" s="3">
-        <f>(K12/G12)+(K12/C12)</f>
-        <v>22.362095503392201</v>
-      </c>
-      <c r="N12" s="3">
-        <f>((K12/G12)+(K12/C12*B12))</f>
-        <v>6290.2433408301213</v>
-      </c>
-      <c r="P12" s="42">
-        <f t="shared" si="0"/>
-        <v>10.02275</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="39">
-        <v>232</v>
-      </c>
-      <c r="C13" s="40">
-        <v>161.5</v>
-      </c>
-      <c r="D13">
-        <v>0.12620000000000001</v>
-      </c>
-      <c r="E13">
-        <v>-13.6877</v>
-      </c>
-      <c r="F13" s="3">
-        <v>504097.78125</v>
-      </c>
-      <c r="G13" s="40">
-        <v>551.25</v>
-      </c>
-      <c r="H13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13">
-        <v>1.387</v>
-      </c>
-      <c r="J13" s="3">
-        <v>2206.9</v>
-      </c>
-      <c r="K13" s="40">
-        <f>F13/B13</f>
-        <v>2172.8352640086205</v>
-      </c>
-      <c r="L13" s="3">
-        <f>(K13/G13)+(K13/E13)</f>
-        <v>-154.80198454707181</v>
-      </c>
-      <c r="M13" s="3">
-        <f>(K13/G13)+(K13/C13)</f>
-        <v>17.395739594612799</v>
-      </c>
-      <c r="N13" s="3">
-        <f>((K13/G13)+(K13/C13*B13))</f>
-        <v>3125.2901419846517</v>
-      </c>
-      <c r="P13" s="42">
-        <f t="shared" si="0"/>
-        <v>2.7562500000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="39">
-        <v>237</v>
-      </c>
-      <c r="C14" s="40">
-        <v>78.3</v>
-      </c>
-      <c r="D14">
-        <v>8.48E-2</v>
-      </c>
-      <c r="E14">
-        <v>-16.337700000000002</v>
-      </c>
-      <c r="F14" s="3">
-        <v>237987.46875</v>
-      </c>
-      <c r="G14" s="40">
-        <v>816.67</v>
-      </c>
-      <c r="H14" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14">
-        <v>1.1517999999999999</v>
-      </c>
-      <c r="J14" s="3">
-        <v>2747.92</v>
-      </c>
-      <c r="K14" s="40">
-        <f>F14/B14</f>
-        <v>1004.1665348101266</v>
-      </c>
-      <c r="L14" s="3">
-        <f>(K14/G14)+(K14/E14)</f>
-        <v>-60.233565121853182</v>
-      </c>
-      <c r="M14" s="3">
-        <f>(K14/G14)+(K14/C14)</f>
-        <v>14.054191187975901</v>
-      </c>
-      <c r="N14" s="3">
-        <f>((K14/G14)+(K14/C14*B14))</f>
-        <v>3040.6608606029172</v>
-      </c>
-      <c r="P14" s="42">
-        <f t="shared" si="0"/>
-        <v>4.0833499999999994</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="39">
-        <v>293</v>
-      </c>
-      <c r="C15" s="39">
-        <v>112.35</v>
-      </c>
-      <c r="D15">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="E15">
-        <v>-15.7897</v>
-      </c>
-      <c r="F15" s="3">
-        <v>326635.5625</v>
-      </c>
-      <c r="G15" s="39">
-        <v>689.06</v>
-      </c>
-      <c r="H15" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15">
-        <v>0.93610000000000004</v>
-      </c>
-      <c r="J15">
-        <v>2433.35</v>
-      </c>
-      <c r="K15" s="40">
-        <f>F15/B15</f>
-        <v>1114.7971416382252</v>
-      </c>
-      <c r="L15" s="3">
-        <f>(K15/G15)+(K15/E15)</f>
-        <v>-68.98495493514929</v>
-      </c>
-      <c r="M15" s="3">
-        <f>(K15/G15)+(K15/C15)</f>
-        <v>11.540390038012868</v>
-      </c>
-      <c r="N15" s="3">
-        <f>((K15/G15)+(K15/C15*B15))</f>
-        <v>2908.9214791200043</v>
-      </c>
-      <c r="P15" s="42">
-        <f t="shared" si="0"/>
-        <v>3.4452999999999996</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="39">
-        <v>65</v>
-      </c>
-      <c r="C16" s="40">
-        <v>117.45</v>
-      </c>
-      <c r="D16">
-        <v>7.6600000000000001E-2</v>
-      </c>
-      <c r="E16">
-        <v>-18.4603</v>
-      </c>
-      <c r="F16" s="3">
-        <v>56900.1796875</v>
-      </c>
-      <c r="G16" s="40">
-        <v>250.57</v>
-      </c>
-      <c r="H16" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16">
-        <v>0.872</v>
-      </c>
-      <c r="J16" s="3">
-        <v>257.36</v>
-      </c>
-      <c r="K16" s="40">
-        <f>F16/B16</f>
-        <v>875.38737980769235</v>
-      </c>
-      <c r="L16" s="3">
-        <f>(K16/G16)+(K16/E16)</f>
-        <v>-43.926413350374055</v>
-      </c>
-      <c r="M16" s="3">
-        <f>(K16/G16)+(K16/C16)</f>
-        <v>10.946861114660344</v>
-      </c>
-      <c r="N16" s="3">
-        <f>((K16/G16)+(K16/C16*B16))</f>
-        <v>487.956587020938</v>
-      </c>
-      <c r="P16" s="42">
-        <f t="shared" si="0"/>
-        <v>1.25285</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="39">
-        <v>163</v>
-      </c>
-      <c r="C17" s="40">
-        <v>112.35</v>
-      </c>
-      <c r="D17">
-        <v>6.5699999999999995E-2</v>
-      </c>
-      <c r="E17">
-        <v>-18.613099999999999</v>
-      </c>
-      <c r="F17" s="3">
-        <v>99084.421875</v>
-      </c>
-      <c r="G17" s="40">
-        <v>479.35</v>
-      </c>
-      <c r="H17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I17">
-        <v>1.0147999999999999</v>
-      </c>
-      <c r="J17" s="3">
-        <v>675.24</v>
-      </c>
-      <c r="K17" s="40">
-        <f>F17/B17</f>
-        <v>607.87988880368096</v>
-      </c>
-      <c r="L17" s="3">
-        <f>(K17/G17)+(K17/E17)</f>
-        <v>-31.390579185816595</v>
-      </c>
-      <c r="M17" s="3">
-        <f>(K17/G17)+(K17/C17)</f>
-        <v>6.6787246099724218</v>
-      </c>
-      <c r="N17" s="3">
-        <f>((K17/G17)+(K17/C17*B17))</f>
-        <v>883.19445212395829</v>
-      </c>
-      <c r="P17" s="42">
-        <f t="shared" si="0"/>
-        <v>2.3967499999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="39">
-        <v>284</v>
-      </c>
-      <c r="C18" s="41">
-        <v>129.19999999999999</v>
-      </c>
-      <c r="D18">
-        <v>5.2299999999999999E-2</v>
-      </c>
-      <c r="E18">
-        <v>-18.380500000000001</v>
-      </c>
-      <c r="F18" s="3">
-        <v>143452.09375</v>
-      </c>
-      <c r="G18" s="40">
-        <v>512.79</v>
-      </c>
-      <c r="H18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18">
-        <v>0.98119999999999996</v>
-      </c>
-      <c r="J18" s="3">
-        <v>830.57</v>
-      </c>
-      <c r="K18" s="40">
-        <f>F18/B18</f>
-        <v>505.11300616197184</v>
-      </c>
-      <c r="L18" s="3">
-        <f>(K18/G18)+(K18/E18)</f>
-        <v>-26.495888640466895</v>
-      </c>
-      <c r="M18" s="3">
-        <f>(K18/G18)+(K18/C18)</f>
-        <v>4.8945723625861657</v>
-      </c>
-      <c r="N18" s="3">
-        <f>((K18/G18)+(K18/C18*B18))</f>
-        <v>1111.2953521136546</v>
-      </c>
-      <c r="P18" s="42">
-        <f t="shared" si="0"/>
-        <v>2.5639499999999997</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="39">
-        <v>273</v>
-      </c>
-      <c r="C19" s="41">
-        <v>152</v>
-      </c>
-      <c r="D19">
-        <v>4.7800000000000002E-2</v>
-      </c>
-      <c r="E19">
-        <v>-20.896899999999999</v>
-      </c>
-      <c r="F19" s="3">
-        <v>114231.59375</v>
-      </c>
-      <c r="G19" s="40">
-        <v>256.39999999999998</v>
-      </c>
-      <c r="H19" t="s">
-        <v>27</v>
-      </c>
-      <c r="I19">
-        <v>1.2103999999999999</v>
-      </c>
-      <c r="J19" s="3">
-        <v>306</v>
-      </c>
-      <c r="K19" s="40">
-        <f>F19/B19</f>
-        <v>418.43074633699632</v>
-      </c>
-      <c r="L19" s="3">
-        <f>(K19/G19)+(K19/E19)</f>
-        <v>-18.39163468873252</v>
-      </c>
-      <c r="M19" s="3">
-        <f>(K19/G19)+(K19/C19)</f>
-        <v>4.3847790460020661</v>
-      </c>
-      <c r="N19" s="3">
-        <f>((K19/G19)+(K19/C19*B19))</f>
-        <v>753.15558828062717</v>
-      </c>
-      <c r="P19" s="42">
-        <f t="shared" si="0"/>
-        <v>1.2819999999999998</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J23" s="16"/>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K23" s="16"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N19" xr:uid="{D881CB1C-05FC-3146-9C78-C0AA3598EAD0}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N19">
-      <sortCondition descending="1" ref="M1:M19"/>
+  <autoFilter ref="B1:P19" xr:uid="{D881CB1C-05FC-3146-9C78-C0AA3598EAD0}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:P19">
+      <sortCondition descending="1" ref="O1:O19"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>